<commit_message>
Changes to the documents
</commit_message>
<xml_diff>
--- a/Rampage/Rampage Gantt Chart.xlsx
+++ b/Rampage/Rampage Gantt Chart.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FAFA91E-933B-46DD-A49F-95BADC8D0AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCA815E-57D1-4D3D-9719-4DC39268090A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10860" yWindow="360" windowWidth="11640" windowHeight="10824" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11304" yWindow="0" windowWidth="11640" windowHeight="10824" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="85">
   <si>
     <t>Create a Project Schedule in this worksheet.
 Enter title of this project in cell B1. 
@@ -159,9 +159,6 @@
   </si>
   <si>
     <t>Sprint 4</t>
-  </si>
-  <si>
-    <t>Task 1</t>
   </si>
   <si>
     <t>date</t>
@@ -317,6 +314,27 @@
   </si>
   <si>
     <t>Login/Register, HUD Design</t>
+  </si>
+  <si>
+    <t>Complete Game Level</t>
+  </si>
+  <si>
+    <t>Login/Register Functionality</t>
+  </si>
+  <si>
+    <t>HUD Functionality</t>
+  </si>
+  <si>
+    <t>Menus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Character Functionality </t>
+  </si>
+  <si>
+    <t>Leaderboard</t>
+  </si>
+  <si>
+    <t>NPCS/ Building, Main Playing Scene</t>
   </si>
 </sst>
 </file>
@@ -725,7 +743,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -969,6 +987,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="12" applyFont="1" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="2" xfId="10" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1974,11 +2001,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DB54"/>
+  <dimension ref="A1:DB61"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" view="pageBreakPreview" zoomScale="59" zoomScaleNormal="110" zoomScaleSheetLayoutView="59" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D38" sqref="D38"/>
+      <pane ySplit="6" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2017,7 +2044,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="58" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -2038,166 +2065,166 @@
         <v>2</v>
       </c>
       <c r="B3" s="60"/>
-      <c r="C3" s="90" t="s">
+      <c r="C3" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="91"/>
-      <c r="E3" s="89">
+      <c r="D3" s="94"/>
+      <c r="E3" s="92">
         <v>45159</v>
       </c>
-      <c r="F3" s="89"/>
+      <c r="F3" s="92"/>
     </row>
     <row r="4" spans="1:106" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="90" t="s">
+      <c r="C4" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="91"/>
+      <c r="D4" s="94"/>
       <c r="E4" s="6">
         <v>1</v>
       </c>
-      <c r="I4" s="86">
+      <c r="I4" s="89">
         <f>I5</f>
         <v>45159</v>
       </c>
-      <c r="J4" s="87"/>
-      <c r="K4" s="87"/>
-      <c r="L4" s="87"/>
-      <c r="M4" s="87"/>
-      <c r="N4" s="87"/>
-      <c r="O4" s="88"/>
-      <c r="P4" s="86">
+      <c r="J4" s="90"/>
+      <c r="K4" s="90"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="90"/>
+      <c r="N4" s="90"/>
+      <c r="O4" s="91"/>
+      <c r="P4" s="89">
         <f>P5</f>
         <v>45166</v>
       </c>
-      <c r="Q4" s="87"/>
-      <c r="R4" s="87"/>
-      <c r="S4" s="87"/>
-      <c r="T4" s="87"/>
-      <c r="U4" s="87"/>
-      <c r="V4" s="88"/>
-      <c r="W4" s="86">
+      <c r="Q4" s="90"/>
+      <c r="R4" s="90"/>
+      <c r="S4" s="90"/>
+      <c r="T4" s="90"/>
+      <c r="U4" s="90"/>
+      <c r="V4" s="91"/>
+      <c r="W4" s="89">
         <f>W5</f>
         <v>45173</v>
       </c>
-      <c r="X4" s="87"/>
-      <c r="Y4" s="87"/>
-      <c r="Z4" s="87"/>
-      <c r="AA4" s="87"/>
-      <c r="AB4" s="87"/>
-      <c r="AC4" s="88"/>
-      <c r="AD4" s="86">
+      <c r="X4" s="90"/>
+      <c r="Y4" s="90"/>
+      <c r="Z4" s="90"/>
+      <c r="AA4" s="90"/>
+      <c r="AB4" s="90"/>
+      <c r="AC4" s="91"/>
+      <c r="AD4" s="89">
         <f>AD5</f>
         <v>45180</v>
       </c>
-      <c r="AE4" s="87"/>
-      <c r="AF4" s="87"/>
-      <c r="AG4" s="87"/>
-      <c r="AH4" s="87"/>
-      <c r="AI4" s="87"/>
-      <c r="AJ4" s="88"/>
-      <c r="AK4" s="86">
+      <c r="AE4" s="90"/>
+      <c r="AF4" s="90"/>
+      <c r="AG4" s="90"/>
+      <c r="AH4" s="90"/>
+      <c r="AI4" s="90"/>
+      <c r="AJ4" s="91"/>
+      <c r="AK4" s="89">
         <f>AK5</f>
         <v>45187</v>
       </c>
-      <c r="AL4" s="87"/>
-      <c r="AM4" s="87"/>
-      <c r="AN4" s="87"/>
-      <c r="AO4" s="87"/>
-      <c r="AP4" s="87"/>
-      <c r="AQ4" s="88"/>
-      <c r="AR4" s="86">
+      <c r="AL4" s="90"/>
+      <c r="AM4" s="90"/>
+      <c r="AN4" s="90"/>
+      <c r="AO4" s="90"/>
+      <c r="AP4" s="90"/>
+      <c r="AQ4" s="91"/>
+      <c r="AR4" s="89">
         <f>AR5</f>
         <v>45194</v>
       </c>
-      <c r="AS4" s="87"/>
-      <c r="AT4" s="87"/>
-      <c r="AU4" s="87"/>
-      <c r="AV4" s="87"/>
-      <c r="AW4" s="87"/>
-      <c r="AX4" s="88"/>
-      <c r="AY4" s="86">
+      <c r="AS4" s="90"/>
+      <c r="AT4" s="90"/>
+      <c r="AU4" s="90"/>
+      <c r="AV4" s="90"/>
+      <c r="AW4" s="90"/>
+      <c r="AX4" s="91"/>
+      <c r="AY4" s="89">
         <f>AY5</f>
         <v>45201</v>
       </c>
-      <c r="AZ4" s="87"/>
-      <c r="BA4" s="87"/>
-      <c r="BB4" s="87"/>
-      <c r="BC4" s="87"/>
-      <c r="BD4" s="87"/>
-      <c r="BE4" s="88"/>
-      <c r="BF4" s="86">
+      <c r="AZ4" s="90"/>
+      <c r="BA4" s="90"/>
+      <c r="BB4" s="90"/>
+      <c r="BC4" s="90"/>
+      <c r="BD4" s="90"/>
+      <c r="BE4" s="91"/>
+      <c r="BF4" s="89">
         <f>BF5</f>
         <v>45208</v>
       </c>
-      <c r="BG4" s="87"/>
-      <c r="BH4" s="87"/>
-      <c r="BI4" s="87"/>
-      <c r="BJ4" s="87"/>
-      <c r="BK4" s="87"/>
-      <c r="BL4" s="88"/>
-      <c r="BM4" s="86">
+      <c r="BG4" s="90"/>
+      <c r="BH4" s="90"/>
+      <c r="BI4" s="90"/>
+      <c r="BJ4" s="90"/>
+      <c r="BK4" s="90"/>
+      <c r="BL4" s="91"/>
+      <c r="BM4" s="89">
         <f>BM5</f>
         <v>45215</v>
       </c>
-      <c r="BN4" s="87"/>
-      <c r="BO4" s="87"/>
-      <c r="BP4" s="87"/>
-      <c r="BQ4" s="87"/>
-      <c r="BR4" s="87"/>
-      <c r="BS4" s="88"/>
-      <c r="BT4" s="86">
+      <c r="BN4" s="90"/>
+      <c r="BO4" s="90"/>
+      <c r="BP4" s="90"/>
+      <c r="BQ4" s="90"/>
+      <c r="BR4" s="90"/>
+      <c r="BS4" s="91"/>
+      <c r="BT4" s="89">
         <f>BT5</f>
         <v>45222</v>
       </c>
-      <c r="BU4" s="87"/>
-      <c r="BV4" s="87"/>
-      <c r="BW4" s="87"/>
-      <c r="BX4" s="87"/>
-      <c r="BY4" s="87"/>
-      <c r="BZ4" s="88"/>
-      <c r="CA4" s="86">
+      <c r="BU4" s="90"/>
+      <c r="BV4" s="90"/>
+      <c r="BW4" s="90"/>
+      <c r="BX4" s="90"/>
+      <c r="BY4" s="90"/>
+      <c r="BZ4" s="91"/>
+      <c r="CA4" s="89">
         <f>CA5</f>
         <v>45229</v>
       </c>
-      <c r="CB4" s="87"/>
-      <c r="CC4" s="87"/>
-      <c r="CD4" s="87"/>
-      <c r="CE4" s="87"/>
-      <c r="CF4" s="87"/>
-      <c r="CG4" s="88"/>
-      <c r="CH4" s="86">
+      <c r="CB4" s="90"/>
+      <c r="CC4" s="90"/>
+      <c r="CD4" s="90"/>
+      <c r="CE4" s="90"/>
+      <c r="CF4" s="90"/>
+      <c r="CG4" s="91"/>
+      <c r="CH4" s="89">
         <f>CH5</f>
         <v>45236</v>
       </c>
-      <c r="CI4" s="87"/>
-      <c r="CJ4" s="87"/>
-      <c r="CK4" s="87"/>
-      <c r="CL4" s="87"/>
-      <c r="CM4" s="87"/>
-      <c r="CN4" s="88"/>
-      <c r="CO4" s="86">
+      <c r="CI4" s="90"/>
+      <c r="CJ4" s="90"/>
+      <c r="CK4" s="90"/>
+      <c r="CL4" s="90"/>
+      <c r="CM4" s="90"/>
+      <c r="CN4" s="91"/>
+      <c r="CO4" s="89">
         <f>CO5</f>
         <v>45243</v>
       </c>
-      <c r="CP4" s="87"/>
-      <c r="CQ4" s="87"/>
-      <c r="CR4" s="87"/>
-      <c r="CS4" s="87"/>
-      <c r="CT4" s="87"/>
-      <c r="CU4" s="88"/>
-      <c r="CV4" s="86">
+      <c r="CP4" s="90"/>
+      <c r="CQ4" s="90"/>
+      <c r="CR4" s="90"/>
+      <c r="CS4" s="90"/>
+      <c r="CT4" s="90"/>
+      <c r="CU4" s="91"/>
+      <c r="CV4" s="89">
         <f>CV5</f>
         <v>45250</v>
       </c>
-      <c r="CW4" s="87"/>
-      <c r="CX4" s="87"/>
-      <c r="CY4" s="87"/>
-      <c r="CZ4" s="87"/>
-      <c r="DA4" s="87"/>
-      <c r="DB4" s="88"/>
+      <c r="CW4" s="90"/>
+      <c r="CX4" s="90"/>
+      <c r="CY4" s="90"/>
+      <c r="CZ4" s="90"/>
+      <c r="DA4" s="90"/>
+      <c r="DB4" s="91"/>
     </row>
     <row r="5" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="56" t="s">
@@ -3140,7 +3167,7 @@
       <c r="F8" s="18"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14" t="str">
-        <f t="shared" ref="H8:H50" si="37">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H57" si="37">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="41"/>
@@ -3247,10 +3274,10 @@
         <v>17</v>
       </c>
       <c r="B9" s="74" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="67" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D9" s="19">
         <v>1</v>
@@ -3372,10 +3399,10 @@
         <v>18</v>
       </c>
       <c r="B10" s="74" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="67" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D10" s="19">
         <v>1</v>
@@ -3495,10 +3522,10 @@
     <row r="11" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="55"/>
       <c r="B11" s="74" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" s="67" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11" s="19">
         <v>1</v>
@@ -3618,10 +3645,10 @@
     <row r="12" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="55"/>
       <c r="B12" s="74" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="67" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D12" s="19">
         <v>1</v>
@@ -4075,10 +4102,10 @@
     <row r="16" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="56"/>
       <c r="B16" s="75" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="83" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D16" s="24">
         <v>1</v>
@@ -4198,10 +4225,10 @@
     <row r="17" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="55"/>
       <c r="B17" s="75" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" s="83" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D17" s="24">
         <v>1</v>
@@ -4321,10 +4348,10 @@
     <row r="18" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="55"/>
       <c r="B18" s="75" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C18" s="69" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D18" s="24">
         <v>1</v>
@@ -4444,10 +4471,10 @@
     <row r="19" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="55"/>
       <c r="B19" s="75" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" s="69" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D19" s="24">
         <v>1</v>
@@ -4567,10 +4594,10 @@
     <row r="20" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="55"/>
       <c r="B20" s="75" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C20" s="69" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D20" s="24">
         <v>1</v>
@@ -4692,10 +4719,10 @@
         <v>23</v>
       </c>
       <c r="B21" s="75" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C21" s="69" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D21" s="24">
         <v>1</v>
@@ -4815,10 +4842,10 @@
     <row r="22" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="55"/>
       <c r="B22" s="75" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22" s="69" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D22" s="24">
         <v>1</v>
@@ -4938,10 +4965,10 @@
     <row r="23" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="55"/>
       <c r="B23" s="75" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C23" s="69" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D23" s="24">
         <v>1</v>
@@ -5061,10 +5088,10 @@
     <row r="24" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="55"/>
       <c r="B24" s="75" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" s="69" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D24" s="24">
         <v>1</v>
@@ -5184,10 +5211,10 @@
     <row r="25" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="55"/>
       <c r="B25" s="75" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" s="69" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D25" s="24">
         <v>1</v>
@@ -5307,10 +5334,10 @@
     <row r="26" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="55"/>
       <c r="B26" s="75" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" s="69" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D26" s="24">
         <v>1</v>
@@ -5765,16 +5792,16 @@
     </row>
     <row r="30" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="76" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C30" s="84" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D30" s="29">
         <v>1</v>
       </c>
       <c r="E30" s="63">
-        <f t="shared" ref="E30:E37" si="40">Project_Start+ 63</f>
+        <f>E46</f>
         <v>45222</v>
       </c>
       <c r="F30" s="63">
@@ -5887,16 +5914,16 @@
     </row>
     <row r="31" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="76" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C31" s="84" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D31" s="29">
         <v>1</v>
       </c>
       <c r="E31" s="63">
-        <f t="shared" si="40"/>
+        <f t="shared" ref="E31:E37" si="40">Project_Start+ 63</f>
         <v>45222</v>
       </c>
       <c r="F31" s="63">
@@ -6009,10 +6036,10 @@
     </row>
     <row r="32" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="76" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C32" s="84" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D32" s="29">
         <v>1</v>
@@ -6131,10 +6158,10 @@
     </row>
     <row r="33" spans="2:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="85" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" s="84" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D33" s="29">
         <v>1</v>
@@ -6250,10 +6277,10 @@
     </row>
     <row r="34" spans="2:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="85" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C34" s="84" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D34" s="29">
         <v>1</v>
@@ -6372,10 +6399,10 @@
     </row>
     <row r="35" spans="2:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="85" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C35" s="84" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D35" s="29">
         <v>1</v>
@@ -6491,10 +6518,10 @@
     </row>
     <row r="36" spans="2:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="85" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C36" s="84" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D36" s="29">
         <v>1</v>
@@ -6610,10 +6637,10 @@
     </row>
     <row r="37" spans="2:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B37" s="85" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C37" s="84" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D37" s="29">
         <v>1</v>
@@ -6729,10 +6756,10 @@
     </row>
     <row r="38" spans="2:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="85" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C38" s="84" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D38" s="29">
         <v>1</v>
@@ -6848,10 +6875,10 @@
     </row>
     <row r="39" spans="2:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" s="85" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C39" s="84" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D39" s="29">
         <v>0.4</v>
@@ -6967,10 +6994,10 @@
     </row>
     <row r="40" spans="2:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B40" s="85" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C40" s="84" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D40" s="29">
         <v>1</v>
@@ -7086,10 +7113,10 @@
     </row>
     <row r="41" spans="2:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B41" s="85" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C41" s="84" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D41" s="29">
         <v>0.5</v>
@@ -7205,10 +7232,10 @@
     </row>
     <row r="42" spans="2:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B42" s="85" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C42" s="84" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D42" s="29">
         <v>0.4</v>
@@ -7649,21 +7676,27 @@
       <c r="DB45" s="41"/>
     </row>
     <row r="46" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="77" t="s">
-        <v>28</v>
-      </c>
-      <c r="C46" s="72"/>
-      <c r="D46" s="34"/>
-      <c r="E46" s="64" t="s">
-        <v>29</v>
-      </c>
-      <c r="F46" s="64" t="s">
-        <v>29</v>
+      <c r="B46" s="86" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" s="87" t="s">
+        <v>51</v>
+      </c>
+      <c r="D46" s="34">
+        <v>1</v>
+      </c>
+      <c r="E46" s="88">
+        <f>Project_Start+ 63</f>
+        <v>45222</v>
+      </c>
+      <c r="F46" s="88">
+        <f>E46+35</f>
+        <v>45257</v>
       </c>
       <c r="G46" s="14"/>
-      <c r="H46" s="14" t="e">
+      <c r="H46" s="14">
         <f t="shared" si="37"/>
-        <v>#VALUE!</v>
+        <v>36</v>
       </c>
       <c r="I46" s="41"/>
       <c r="J46" s="41"/>
@@ -7765,22 +7798,19 @@
       <c r="DB46" s="41"/>
     </row>
     <row r="47" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="77" t="s">
-        <v>25</v>
-      </c>
-      <c r="C47" s="72"/>
-      <c r="D47" s="34"/>
-      <c r="E47" s="64" t="s">
-        <v>29</v>
-      </c>
-      <c r="F47" s="64" t="s">
-        <v>29</v>
-      </c>
+      <c r="B47" s="86" t="s">
+        <v>79</v>
+      </c>
+      <c r="C47" s="87" t="s">
+        <v>64</v>
+      </c>
+      <c r="D47" s="34">
+        <v>1</v>
+      </c>
+      <c r="E47" s="64"/>
+      <c r="F47" s="64"/>
       <c r="G47" s="14"/>
-      <c r="H47" s="14" t="e">
-        <f t="shared" si="37"/>
-        <v>#VALUE!</v>
-      </c>
+      <c r="H47" s="14"/>
       <c r="I47" s="41"/>
       <c r="J47" s="41"/>
       <c r="K47" s="41"/>
@@ -7881,22 +7911,19 @@
       <c r="DB47" s="41"/>
     </row>
     <row r="48" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="77" t="s">
-        <v>26</v>
-      </c>
-      <c r="C48" s="72"/>
-      <c r="D48" s="34"/>
-      <c r="E48" s="64" t="s">
-        <v>29</v>
-      </c>
-      <c r="F48" s="64" t="s">
-        <v>29</v>
-      </c>
+      <c r="B48" s="86" t="s">
+        <v>80</v>
+      </c>
+      <c r="C48" s="87" t="s">
+        <v>64</v>
+      </c>
+      <c r="D48" s="34">
+        <v>0.2</v>
+      </c>
+      <c r="E48" s="64"/>
+      <c r="F48" s="64"/>
       <c r="G48" s="14"/>
-      <c r="H48" s="14" t="e">
-        <f t="shared" si="37"/>
-        <v>#VALUE!</v>
-      </c>
+      <c r="H48" s="14"/>
       <c r="I48" s="41"/>
       <c r="J48" s="41"/>
       <c r="K48" s="41"/>
@@ -7997,22 +8024,19 @@
       <c r="DB48" s="41"/>
     </row>
     <row r="49" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="77" t="s">
-        <v>19</v>
-      </c>
-      <c r="C49" s="72"/>
-      <c r="D49" s="34"/>
-      <c r="E49" s="64" t="s">
-        <v>29</v>
-      </c>
-      <c r="F49" s="64" t="s">
-        <v>29</v>
-      </c>
+      <c r="B49" s="86" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" s="87" t="s">
+        <v>65</v>
+      </c>
+      <c r="D49" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="E49" s="64"/>
+      <c r="F49" s="64"/>
       <c r="G49" s="14"/>
-      <c r="H49" s="14" t="e">
-        <f t="shared" si="37"/>
-        <v>#VALUE!</v>
-      </c>
+      <c r="H49" s="14"/>
       <c r="I49" s="41"/>
       <c r="J49" s="41"/>
       <c r="K49" s="41"/>
@@ -8113,22 +8137,19 @@
       <c r="DB49" s="41"/>
     </row>
     <row r="50" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="77" t="s">
-        <v>20</v>
-      </c>
-      <c r="C50" s="72"/>
-      <c r="D50" s="34"/>
-      <c r="E50" s="64" t="s">
-        <v>29</v>
-      </c>
-      <c r="F50" s="64" t="s">
-        <v>29</v>
-      </c>
+      <c r="B50" s="86" t="s">
+        <v>82</v>
+      </c>
+      <c r="C50" s="87" t="s">
+        <v>62</v>
+      </c>
+      <c r="D50" s="34">
+        <v>0.6</v>
+      </c>
+      <c r="E50" s="64"/>
+      <c r="F50" s="64"/>
       <c r="G50" s="14"/>
-      <c r="H50" s="14" t="e">
-        <f t="shared" si="37"/>
-        <v>#VALUE!</v>
-      </c>
+      <c r="H50" s="14"/>
       <c r="I50" s="41"/>
       <c r="J50" s="41"/>
       <c r="K50" s="41"/>
@@ -8228,231 +8249,240 @@
       <c r="DA50" s="41"/>
       <c r="DB50" s="41"/>
     </row>
-    <row r="51" spans="2:106" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
-      <c r="L51" s="3"/>
-      <c r="M51" s="3"/>
-      <c r="N51" s="3"/>
-      <c r="O51" s="3"/>
-      <c r="P51" s="3"/>
-      <c r="Q51" s="3"/>
-      <c r="R51" s="3"/>
-      <c r="S51" s="3"/>
-      <c r="T51" s="3"/>
-      <c r="U51" s="3"/>
-      <c r="V51" s="3"/>
-      <c r="W51" s="3"/>
-      <c r="X51" s="3"/>
-      <c r="Y51" s="3"/>
-      <c r="Z51" s="3"/>
-      <c r="AA51" s="3"/>
-      <c r="AB51" s="3"/>
-      <c r="AC51" s="3"/>
-      <c r="AD51" s="3"/>
-      <c r="AE51" s="3"/>
-      <c r="AF51" s="3"/>
-      <c r="AG51" s="3"/>
-      <c r="AH51" s="3"/>
-      <c r="AI51" s="3"/>
-      <c r="AJ51" s="3"/>
-      <c r="AK51" s="3"/>
-      <c r="AL51" s="3"/>
-      <c r="AM51" s="3"/>
-      <c r="AN51" s="3"/>
-      <c r="AO51" s="3"/>
-      <c r="AP51" s="3"/>
-      <c r="AQ51" s="3"/>
-      <c r="AR51" s="3"/>
-      <c r="AS51" s="3"/>
-      <c r="AT51" s="3"/>
-      <c r="AU51" s="3"/>
-      <c r="AV51" s="3"/>
-      <c r="AW51" s="3"/>
-      <c r="AX51" s="3"/>
-      <c r="AY51" s="3"/>
-      <c r="AZ51" s="3"/>
-      <c r="BA51" s="3"/>
-      <c r="BB51" s="3"/>
-      <c r="BC51" s="3"/>
-      <c r="BD51" s="3"/>
-      <c r="BE51" s="3"/>
-      <c r="BF51" s="3"/>
-      <c r="BG51" s="3"/>
-      <c r="BH51" s="3"/>
-      <c r="BI51" s="3"/>
-      <c r="BJ51" s="3"/>
-      <c r="BK51" s="3"/>
-      <c r="BL51" s="3"/>
-      <c r="BM51" s="3"/>
-      <c r="BN51" s="3"/>
-      <c r="BO51" s="3"/>
-      <c r="BP51" s="3"/>
-      <c r="BQ51" s="3"/>
-      <c r="BR51" s="3"/>
-      <c r="BS51" s="3"/>
-      <c r="BT51" s="3"/>
-      <c r="BU51" s="3"/>
-      <c r="BV51" s="3"/>
-      <c r="BW51" s="3"/>
-      <c r="BX51" s="3"/>
-      <c r="BY51" s="3"/>
-      <c r="BZ51" s="3"/>
-      <c r="CA51" s="3"/>
-      <c r="CB51" s="3"/>
-      <c r="CC51" s="3"/>
-      <c r="CD51" s="3"/>
-      <c r="CE51" s="3"/>
-      <c r="CF51" s="3"/>
-      <c r="CG51" s="3"/>
-      <c r="CH51" s="3"/>
-      <c r="CI51" s="3"/>
-      <c r="CJ51" s="3"/>
-      <c r="CK51" s="3"/>
-      <c r="CL51" s="3"/>
-      <c r="CM51" s="3"/>
-      <c r="CN51" s="3"/>
-      <c r="CO51" s="3"/>
-      <c r="CP51" s="3"/>
-      <c r="CQ51" s="3"/>
-      <c r="CR51" s="3"/>
-      <c r="CS51" s="3"/>
-      <c r="CT51" s="3"/>
-      <c r="CU51" s="3"/>
-      <c r="CV51" s="3"/>
-      <c r="CW51" s="3"/>
-      <c r="CX51" s="3"/>
-      <c r="CY51" s="3"/>
-      <c r="CZ51" s="3"/>
-      <c r="DA51" s="3"/>
-      <c r="DB51" s="3"/>
+    <row r="51" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="86" t="s">
+        <v>83</v>
+      </c>
+      <c r="C51" s="87" t="s">
+        <v>64</v>
+      </c>
+      <c r="D51" s="34">
+        <v>0.9</v>
+      </c>
+      <c r="E51" s="64"/>
+      <c r="F51" s="64"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="41"/>
+      <c r="J51" s="41"/>
+      <c r="K51" s="41"/>
+      <c r="L51" s="41"/>
+      <c r="M51" s="41"/>
+      <c r="N51" s="41"/>
+      <c r="O51" s="41"/>
+      <c r="P51" s="41"/>
+      <c r="Q51" s="41"/>
+      <c r="R51" s="41"/>
+      <c r="S51" s="41"/>
+      <c r="T51" s="41"/>
+      <c r="U51" s="41"/>
+      <c r="V51" s="41"/>
+      <c r="W51" s="41"/>
+      <c r="X51" s="41"/>
+      <c r="Y51" s="41"/>
+      <c r="Z51" s="41"/>
+      <c r="AA51" s="41"/>
+      <c r="AB51" s="41"/>
+      <c r="AC51" s="41"/>
+      <c r="AD51" s="41"/>
+      <c r="AE51" s="41"/>
+      <c r="AF51" s="41"/>
+      <c r="AG51" s="41"/>
+      <c r="AH51" s="41"/>
+      <c r="AI51" s="41"/>
+      <c r="AJ51" s="41"/>
+      <c r="AK51" s="41"/>
+      <c r="AL51" s="41"/>
+      <c r="AM51" s="41"/>
+      <c r="AN51" s="41"/>
+      <c r="AO51" s="41"/>
+      <c r="AP51" s="41"/>
+      <c r="AQ51" s="41"/>
+      <c r="AR51" s="41"/>
+      <c r="AS51" s="41"/>
+      <c r="AT51" s="41"/>
+      <c r="AU51" s="41"/>
+      <c r="AV51" s="41"/>
+      <c r="AW51" s="41"/>
+      <c r="AX51" s="41"/>
+      <c r="AY51" s="41"/>
+      <c r="AZ51" s="41"/>
+      <c r="BA51" s="41"/>
+      <c r="BB51" s="41"/>
+      <c r="BC51" s="41"/>
+      <c r="BD51" s="41"/>
+      <c r="BE51" s="41"/>
+      <c r="BF51" s="41"/>
+      <c r="BG51" s="41"/>
+      <c r="BH51" s="41"/>
+      <c r="BI51" s="41"/>
+      <c r="BJ51" s="41"/>
+      <c r="BK51" s="41"/>
+      <c r="BL51" s="41"/>
+      <c r="BM51" s="41"/>
+      <c r="BN51" s="41"/>
+      <c r="BO51" s="41"/>
+      <c r="BP51" s="41"/>
+      <c r="BQ51" s="41"/>
+      <c r="BR51" s="41"/>
+      <c r="BS51" s="41"/>
+      <c r="BT51" s="41"/>
+      <c r="BU51" s="41"/>
+      <c r="BV51" s="41"/>
+      <c r="BW51" s="41"/>
+      <c r="BX51" s="41"/>
+      <c r="BY51" s="41"/>
+      <c r="BZ51" s="41"/>
+      <c r="CA51" s="41"/>
+      <c r="CB51" s="41"/>
+      <c r="CC51" s="41"/>
+      <c r="CD51" s="41"/>
+      <c r="CE51" s="41"/>
+      <c r="CF51" s="41"/>
+      <c r="CG51" s="41"/>
+      <c r="CH51" s="41"/>
+      <c r="CI51" s="41"/>
+      <c r="CJ51" s="41"/>
+      <c r="CK51" s="41"/>
+      <c r="CL51" s="41"/>
+      <c r="CM51" s="41"/>
+      <c r="CN51" s="41"/>
+      <c r="CO51" s="41"/>
+      <c r="CP51" s="41"/>
+      <c r="CQ51" s="41"/>
+      <c r="CR51" s="41"/>
+      <c r="CS51" s="41"/>
+      <c r="CT51" s="41"/>
+      <c r="CU51" s="41"/>
+      <c r="CV51" s="41"/>
+      <c r="CW51" s="41"/>
+      <c r="CX51" s="41"/>
+      <c r="CY51" s="41"/>
+      <c r="CZ51" s="41"/>
+      <c r="DA51" s="41"/>
+      <c r="DB51" s="41"/>
     </row>
     <row r="52" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
-      <c r="L52" s="3"/>
-      <c r="M52" s="3"/>
-      <c r="N52" s="3"/>
-      <c r="O52" s="3"/>
-      <c r="P52" s="3"/>
-      <c r="Q52" s="3"/>
-      <c r="R52" s="3"/>
-      <c r="S52" s="3"/>
-      <c r="T52" s="3"/>
-      <c r="U52" s="3"/>
-      <c r="V52" s="3"/>
-      <c r="W52" s="3"/>
-      <c r="X52" s="3"/>
-      <c r="Y52" s="3"/>
-      <c r="Z52" s="3"/>
-      <c r="AA52" s="3"/>
-      <c r="AB52" s="3"/>
-      <c r="AC52" s="3"/>
-      <c r="AD52" s="3"/>
-      <c r="AE52" s="3"/>
-      <c r="AF52" s="3"/>
-      <c r="AG52" s="3"/>
-      <c r="AH52" s="3"/>
-      <c r="AI52" s="3"/>
-      <c r="AJ52" s="3"/>
-      <c r="AK52" s="3"/>
-      <c r="AL52" s="3"/>
-      <c r="AM52" s="3"/>
-      <c r="AN52" s="3"/>
-      <c r="AO52" s="3"/>
-      <c r="AP52" s="3"/>
-      <c r="AQ52" s="3"/>
-      <c r="AR52" s="3"/>
-      <c r="AS52" s="3"/>
-      <c r="AT52" s="3"/>
-      <c r="AU52" s="3"/>
-      <c r="AV52" s="3"/>
-      <c r="AW52" s="3"/>
-      <c r="AX52" s="3"/>
-      <c r="AY52" s="3"/>
-      <c r="AZ52" s="3"/>
-      <c r="BA52" s="3"/>
-      <c r="BB52" s="3"/>
-      <c r="BC52" s="3"/>
-      <c r="BD52" s="3"/>
-      <c r="BE52" s="3"/>
-      <c r="BF52" s="3"/>
-      <c r="BG52" s="3"/>
-      <c r="BH52" s="3"/>
-      <c r="BI52" s="3"/>
-      <c r="BJ52" s="3"/>
-      <c r="BK52" s="3"/>
-      <c r="BL52" s="3"/>
-      <c r="BM52" s="3"/>
-      <c r="BN52" s="3"/>
-      <c r="BO52" s="3"/>
-      <c r="BP52" s="3"/>
-      <c r="BQ52" s="3"/>
-      <c r="BR52" s="3"/>
-      <c r="BS52" s="3"/>
-      <c r="BT52" s="3"/>
-      <c r="BU52" s="3"/>
-      <c r="BV52" s="3"/>
-      <c r="BW52" s="3"/>
-      <c r="BX52" s="3"/>
-      <c r="BY52" s="3"/>
-      <c r="BZ52" s="3"/>
-      <c r="CA52" s="3"/>
-      <c r="CB52" s="3"/>
-      <c r="CC52" s="3"/>
-      <c r="CD52" s="3"/>
-      <c r="CE52" s="3"/>
-      <c r="CF52" s="3"/>
-      <c r="CG52" s="3"/>
-      <c r="CH52" s="3"/>
-      <c r="CI52" s="3"/>
-      <c r="CJ52" s="3"/>
-      <c r="CK52" s="3"/>
-      <c r="CL52" s="3"/>
-      <c r="CM52" s="3"/>
-      <c r="CN52" s="3"/>
-      <c r="CO52" s="3"/>
-      <c r="CP52" s="3"/>
-      <c r="CQ52" s="3"/>
-      <c r="CR52" s="3"/>
-      <c r="CS52" s="3"/>
-      <c r="CT52" s="3"/>
-      <c r="CU52" s="3"/>
-      <c r="CV52" s="3"/>
-      <c r="CW52" s="3"/>
-      <c r="CX52" s="3"/>
-      <c r="CY52" s="3"/>
-      <c r="CZ52" s="3"/>
-      <c r="DA52" s="3"/>
-      <c r="DB52" s="3"/>
+      <c r="B52" s="86" t="s">
+        <v>84</v>
+      </c>
+      <c r="C52" s="87" t="s">
+        <v>70</v>
+      </c>
+      <c r="D52" s="34">
+        <v>0.6</v>
+      </c>
+      <c r="E52" s="64"/>
+      <c r="F52" s="64"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="41"/>
+      <c r="J52" s="41"/>
+      <c r="K52" s="41"/>
+      <c r="L52" s="41"/>
+      <c r="M52" s="41"/>
+      <c r="N52" s="41"/>
+      <c r="O52" s="41"/>
+      <c r="P52" s="41"/>
+      <c r="Q52" s="41"/>
+      <c r="R52" s="41"/>
+      <c r="S52" s="41"/>
+      <c r="T52" s="41"/>
+      <c r="U52" s="41"/>
+      <c r="V52" s="41"/>
+      <c r="W52" s="41"/>
+      <c r="X52" s="41"/>
+      <c r="Y52" s="41"/>
+      <c r="Z52" s="41"/>
+      <c r="AA52" s="41"/>
+      <c r="AB52" s="41"/>
+      <c r="AC52" s="41"/>
+      <c r="AD52" s="41"/>
+      <c r="AE52" s="41"/>
+      <c r="AF52" s="41"/>
+      <c r="AG52" s="41"/>
+      <c r="AH52" s="41"/>
+      <c r="AI52" s="41"/>
+      <c r="AJ52" s="41"/>
+      <c r="AK52" s="41"/>
+      <c r="AL52" s="41"/>
+      <c r="AM52" s="41"/>
+      <c r="AN52" s="41"/>
+      <c r="AO52" s="41"/>
+      <c r="AP52" s="41"/>
+      <c r="AQ52" s="41"/>
+      <c r="AR52" s="41"/>
+      <c r="AS52" s="41"/>
+      <c r="AT52" s="41"/>
+      <c r="AU52" s="41"/>
+      <c r="AV52" s="41"/>
+      <c r="AW52" s="41"/>
+      <c r="AX52" s="41"/>
+      <c r="AY52" s="41"/>
+      <c r="AZ52" s="41"/>
+      <c r="BA52" s="41"/>
+      <c r="BB52" s="41"/>
+      <c r="BC52" s="41"/>
+      <c r="BD52" s="41"/>
+      <c r="BE52" s="41"/>
+      <c r="BF52" s="41"/>
+      <c r="BG52" s="41"/>
+      <c r="BH52" s="41"/>
+      <c r="BI52" s="41"/>
+      <c r="BJ52" s="41"/>
+      <c r="BK52" s="41"/>
+      <c r="BL52" s="41"/>
+      <c r="BM52" s="41"/>
+      <c r="BN52" s="41"/>
+      <c r="BO52" s="41"/>
+      <c r="BP52" s="41"/>
+      <c r="BQ52" s="41"/>
+      <c r="BR52" s="41"/>
+      <c r="BS52" s="41"/>
+      <c r="BT52" s="41"/>
+      <c r="BU52" s="41"/>
+      <c r="BV52" s="41"/>
+      <c r="BW52" s="41"/>
+      <c r="BX52" s="41"/>
+      <c r="BY52" s="41"/>
+      <c r="BZ52" s="41"/>
+      <c r="CA52" s="41"/>
+      <c r="CB52" s="41"/>
+      <c r="CC52" s="41"/>
+      <c r="CD52" s="41"/>
+      <c r="CE52" s="41"/>
+      <c r="CF52" s="41"/>
+      <c r="CG52" s="41"/>
+      <c r="CH52" s="41"/>
+      <c r="CI52" s="41"/>
+      <c r="CJ52" s="41"/>
+      <c r="CK52" s="41"/>
+      <c r="CL52" s="41"/>
+      <c r="CM52" s="41"/>
+      <c r="CN52" s="41"/>
+      <c r="CO52" s="41"/>
+      <c r="CP52" s="41"/>
+      <c r="CQ52" s="41"/>
+      <c r="CR52" s="41"/>
+      <c r="CS52" s="41"/>
+      <c r="CT52" s="41"/>
+      <c r="CU52" s="41"/>
+      <c r="CV52" s="41"/>
+      <c r="CW52" s="41"/>
+      <c r="CX52" s="41"/>
+      <c r="CY52" s="41"/>
+      <c r="CZ52" s="41"/>
+      <c r="DA52" s="41"/>
+      <c r="DB52" s="41"/>
     </row>
     <row r="53" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="78"/>
-      <c r="C53" s="73"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="65"/>
-      <c r="F53" s="65"/>
+      <c r="B53" s="77"/>
+      <c r="C53" s="72"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="64"/>
+      <c r="F53" s="64"/>
       <c r="G53" s="14"/>
-      <c r="H53" s="14" t="str">
-        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
-        <v/>
-      </c>
+      <c r="H53" s="14"/>
       <c r="I53" s="41"/>
       <c r="J53" s="41"/>
       <c r="K53" s="41"/>
@@ -8553,116 +8583,904 @@
       <c r="DB53" s="41"/>
     </row>
     <row r="54" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="C54" s="36"/>
-      <c r="D54" s="37"/>
-      <c r="E54" s="38"/>
-      <c r="F54" s="39"/>
-      <c r="G54" s="40"/>
-      <c r="H54" s="40" t="str">
+      <c r="B54" s="77" t="s">
+        <v>25</v>
+      </c>
+      <c r="C54" s="72"/>
+      <c r="D54" s="34"/>
+      <c r="E54" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="F54" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14" t="e">
+        <f t="shared" si="37"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I54" s="41"/>
+      <c r="J54" s="41"/>
+      <c r="K54" s="41"/>
+      <c r="L54" s="41"/>
+      <c r="M54" s="41"/>
+      <c r="N54" s="41"/>
+      <c r="O54" s="41"/>
+      <c r="P54" s="41"/>
+      <c r="Q54" s="41"/>
+      <c r="R54" s="41"/>
+      <c r="S54" s="41"/>
+      <c r="T54" s="41"/>
+      <c r="U54" s="41"/>
+      <c r="V54" s="41"/>
+      <c r="W54" s="41"/>
+      <c r="X54" s="41"/>
+      <c r="Y54" s="41"/>
+      <c r="Z54" s="41"/>
+      <c r="AA54" s="41"/>
+      <c r="AB54" s="41"/>
+      <c r="AC54" s="41"/>
+      <c r="AD54" s="41"/>
+      <c r="AE54" s="41"/>
+      <c r="AF54" s="41"/>
+      <c r="AG54" s="41"/>
+      <c r="AH54" s="41"/>
+      <c r="AI54" s="41"/>
+      <c r="AJ54" s="41"/>
+      <c r="AK54" s="41"/>
+      <c r="AL54" s="41"/>
+      <c r="AM54" s="41"/>
+      <c r="AN54" s="41"/>
+      <c r="AO54" s="41"/>
+      <c r="AP54" s="41"/>
+      <c r="AQ54" s="41"/>
+      <c r="AR54" s="41"/>
+      <c r="AS54" s="41"/>
+      <c r="AT54" s="41"/>
+      <c r="AU54" s="41"/>
+      <c r="AV54" s="41"/>
+      <c r="AW54" s="41"/>
+      <c r="AX54" s="41"/>
+      <c r="AY54" s="41"/>
+      <c r="AZ54" s="41"/>
+      <c r="BA54" s="41"/>
+      <c r="BB54" s="41"/>
+      <c r="BC54" s="41"/>
+      <c r="BD54" s="41"/>
+      <c r="BE54" s="41"/>
+      <c r="BF54" s="41"/>
+      <c r="BG54" s="41"/>
+      <c r="BH54" s="41"/>
+      <c r="BI54" s="41"/>
+      <c r="BJ54" s="41"/>
+      <c r="BK54" s="41"/>
+      <c r="BL54" s="41"/>
+      <c r="BM54" s="41"/>
+      <c r="BN54" s="41"/>
+      <c r="BO54" s="41"/>
+      <c r="BP54" s="41"/>
+      <c r="BQ54" s="41"/>
+      <c r="BR54" s="41"/>
+      <c r="BS54" s="41"/>
+      <c r="BT54" s="41"/>
+      <c r="BU54" s="41"/>
+      <c r="BV54" s="41"/>
+      <c r="BW54" s="41"/>
+      <c r="BX54" s="41"/>
+      <c r="BY54" s="41"/>
+      <c r="BZ54" s="41"/>
+      <c r="CA54" s="41"/>
+      <c r="CB54" s="41"/>
+      <c r="CC54" s="41"/>
+      <c r="CD54" s="41"/>
+      <c r="CE54" s="41"/>
+      <c r="CF54" s="41"/>
+      <c r="CG54" s="41"/>
+      <c r="CH54" s="41"/>
+      <c r="CI54" s="41"/>
+      <c r="CJ54" s="41"/>
+      <c r="CK54" s="41"/>
+      <c r="CL54" s="41"/>
+      <c r="CM54" s="41"/>
+      <c r="CN54" s="41"/>
+      <c r="CO54" s="41"/>
+      <c r="CP54" s="41"/>
+      <c r="CQ54" s="41"/>
+      <c r="CR54" s="41"/>
+      <c r="CS54" s="41"/>
+      <c r="CT54" s="41"/>
+      <c r="CU54" s="41"/>
+      <c r="CV54" s="41"/>
+      <c r="CW54" s="41"/>
+      <c r="CX54" s="41"/>
+      <c r="CY54" s="41"/>
+      <c r="CZ54" s="41"/>
+      <c r="DA54" s="41"/>
+      <c r="DB54" s="41"/>
+    </row>
+    <row r="55" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B55" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="C55" s="72"/>
+      <c r="D55" s="34"/>
+      <c r="E55" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="F55" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14" t="e">
+        <f t="shared" si="37"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I55" s="41"/>
+      <c r="J55" s="41"/>
+      <c r="K55" s="41"/>
+      <c r="L55" s="41"/>
+      <c r="M55" s="41"/>
+      <c r="N55" s="41"/>
+      <c r="O55" s="41"/>
+      <c r="P55" s="41"/>
+      <c r="Q55" s="41"/>
+      <c r="R55" s="41"/>
+      <c r="S55" s="41"/>
+      <c r="T55" s="41"/>
+      <c r="U55" s="41"/>
+      <c r="V55" s="41"/>
+      <c r="W55" s="41"/>
+      <c r="X55" s="41"/>
+      <c r="Y55" s="41"/>
+      <c r="Z55" s="41"/>
+      <c r="AA55" s="41"/>
+      <c r="AB55" s="41"/>
+      <c r="AC55" s="41"/>
+      <c r="AD55" s="41"/>
+      <c r="AE55" s="41"/>
+      <c r="AF55" s="41"/>
+      <c r="AG55" s="41"/>
+      <c r="AH55" s="41"/>
+      <c r="AI55" s="41"/>
+      <c r="AJ55" s="41"/>
+      <c r="AK55" s="41"/>
+      <c r="AL55" s="41"/>
+      <c r="AM55" s="41"/>
+      <c r="AN55" s="41"/>
+      <c r="AO55" s="41"/>
+      <c r="AP55" s="41"/>
+      <c r="AQ55" s="41"/>
+      <c r="AR55" s="41"/>
+      <c r="AS55" s="41"/>
+      <c r="AT55" s="41"/>
+      <c r="AU55" s="41"/>
+      <c r="AV55" s="41"/>
+      <c r="AW55" s="41"/>
+      <c r="AX55" s="41"/>
+      <c r="AY55" s="41"/>
+      <c r="AZ55" s="41"/>
+      <c r="BA55" s="41"/>
+      <c r="BB55" s="41"/>
+      <c r="BC55" s="41"/>
+      <c r="BD55" s="41"/>
+      <c r="BE55" s="41"/>
+      <c r="BF55" s="41"/>
+      <c r="BG55" s="41"/>
+      <c r="BH55" s="41"/>
+      <c r="BI55" s="41"/>
+      <c r="BJ55" s="41"/>
+      <c r="BK55" s="41"/>
+      <c r="BL55" s="41"/>
+      <c r="BM55" s="41"/>
+      <c r="BN55" s="41"/>
+      <c r="BO55" s="41"/>
+      <c r="BP55" s="41"/>
+      <c r="BQ55" s="41"/>
+      <c r="BR55" s="41"/>
+      <c r="BS55" s="41"/>
+      <c r="BT55" s="41"/>
+      <c r="BU55" s="41"/>
+      <c r="BV55" s="41"/>
+      <c r="BW55" s="41"/>
+      <c r="BX55" s="41"/>
+      <c r="BY55" s="41"/>
+      <c r="BZ55" s="41"/>
+      <c r="CA55" s="41"/>
+      <c r="CB55" s="41"/>
+      <c r="CC55" s="41"/>
+      <c r="CD55" s="41"/>
+      <c r="CE55" s="41"/>
+      <c r="CF55" s="41"/>
+      <c r="CG55" s="41"/>
+      <c r="CH55" s="41"/>
+      <c r="CI55" s="41"/>
+      <c r="CJ55" s="41"/>
+      <c r="CK55" s="41"/>
+      <c r="CL55" s="41"/>
+      <c r="CM55" s="41"/>
+      <c r="CN55" s="41"/>
+      <c r="CO55" s="41"/>
+      <c r="CP55" s="41"/>
+      <c r="CQ55" s="41"/>
+      <c r="CR55" s="41"/>
+      <c r="CS55" s="41"/>
+      <c r="CT55" s="41"/>
+      <c r="CU55" s="41"/>
+      <c r="CV55" s="41"/>
+      <c r="CW55" s="41"/>
+      <c r="CX55" s="41"/>
+      <c r="CY55" s="41"/>
+      <c r="CZ55" s="41"/>
+      <c r="DA55" s="41"/>
+      <c r="DB55" s="41"/>
+    </row>
+    <row r="56" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B56" s="77" t="s">
+        <v>19</v>
+      </c>
+      <c r="C56" s="72"/>
+      <c r="D56" s="34"/>
+      <c r="E56" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="F56" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14" t="e">
+        <f t="shared" si="37"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I56" s="41"/>
+      <c r="J56" s="41"/>
+      <c r="K56" s="41"/>
+      <c r="L56" s="41"/>
+      <c r="M56" s="41"/>
+      <c r="N56" s="41"/>
+      <c r="O56" s="41"/>
+      <c r="P56" s="41"/>
+      <c r="Q56" s="41"/>
+      <c r="R56" s="41"/>
+      <c r="S56" s="41"/>
+      <c r="T56" s="41"/>
+      <c r="U56" s="41"/>
+      <c r="V56" s="41"/>
+      <c r="W56" s="41"/>
+      <c r="X56" s="41"/>
+      <c r="Y56" s="41"/>
+      <c r="Z56" s="41"/>
+      <c r="AA56" s="41"/>
+      <c r="AB56" s="41"/>
+      <c r="AC56" s="41"/>
+      <c r="AD56" s="41"/>
+      <c r="AE56" s="41"/>
+      <c r="AF56" s="41"/>
+      <c r="AG56" s="41"/>
+      <c r="AH56" s="41"/>
+      <c r="AI56" s="41"/>
+      <c r="AJ56" s="41"/>
+      <c r="AK56" s="41"/>
+      <c r="AL56" s="41"/>
+      <c r="AM56" s="41"/>
+      <c r="AN56" s="41"/>
+      <c r="AO56" s="41"/>
+      <c r="AP56" s="41"/>
+      <c r="AQ56" s="41"/>
+      <c r="AR56" s="41"/>
+      <c r="AS56" s="41"/>
+      <c r="AT56" s="41"/>
+      <c r="AU56" s="41"/>
+      <c r="AV56" s="41"/>
+      <c r="AW56" s="41"/>
+      <c r="AX56" s="41"/>
+      <c r="AY56" s="41"/>
+      <c r="AZ56" s="41"/>
+      <c r="BA56" s="41"/>
+      <c r="BB56" s="41"/>
+      <c r="BC56" s="41"/>
+      <c r="BD56" s="41"/>
+      <c r="BE56" s="41"/>
+      <c r="BF56" s="41"/>
+      <c r="BG56" s="41"/>
+      <c r="BH56" s="41"/>
+      <c r="BI56" s="41"/>
+      <c r="BJ56" s="41"/>
+      <c r="BK56" s="41"/>
+      <c r="BL56" s="41"/>
+      <c r="BM56" s="41"/>
+      <c r="BN56" s="41"/>
+      <c r="BO56" s="41"/>
+      <c r="BP56" s="41"/>
+      <c r="BQ56" s="41"/>
+      <c r="BR56" s="41"/>
+      <c r="BS56" s="41"/>
+      <c r="BT56" s="41"/>
+      <c r="BU56" s="41"/>
+      <c r="BV56" s="41"/>
+      <c r="BW56" s="41"/>
+      <c r="BX56" s="41"/>
+      <c r="BY56" s="41"/>
+      <c r="BZ56" s="41"/>
+      <c r="CA56" s="41"/>
+      <c r="CB56" s="41"/>
+      <c r="CC56" s="41"/>
+      <c r="CD56" s="41"/>
+      <c r="CE56" s="41"/>
+      <c r="CF56" s="41"/>
+      <c r="CG56" s="41"/>
+      <c r="CH56" s="41"/>
+      <c r="CI56" s="41"/>
+      <c r="CJ56" s="41"/>
+      <c r="CK56" s="41"/>
+      <c r="CL56" s="41"/>
+      <c r="CM56" s="41"/>
+      <c r="CN56" s="41"/>
+      <c r="CO56" s="41"/>
+      <c r="CP56" s="41"/>
+      <c r="CQ56" s="41"/>
+      <c r="CR56" s="41"/>
+      <c r="CS56" s="41"/>
+      <c r="CT56" s="41"/>
+      <c r="CU56" s="41"/>
+      <c r="CV56" s="41"/>
+      <c r="CW56" s="41"/>
+      <c r="CX56" s="41"/>
+      <c r="CY56" s="41"/>
+      <c r="CZ56" s="41"/>
+      <c r="DA56" s="41"/>
+      <c r="DB56" s="41"/>
+    </row>
+    <row r="57" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B57" s="77" t="s">
+        <v>20</v>
+      </c>
+      <c r="C57" s="72"/>
+      <c r="D57" s="34"/>
+      <c r="E57" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="F57" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="G57" s="14"/>
+      <c r="H57" s="14" t="e">
+        <f t="shared" si="37"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I57" s="41"/>
+      <c r="J57" s="41"/>
+      <c r="K57" s="41"/>
+      <c r="L57" s="41"/>
+      <c r="M57" s="41"/>
+      <c r="N57" s="41"/>
+      <c r="O57" s="41"/>
+      <c r="P57" s="41"/>
+      <c r="Q57" s="41"/>
+      <c r="R57" s="41"/>
+      <c r="S57" s="41"/>
+      <c r="T57" s="41"/>
+      <c r="U57" s="41"/>
+      <c r="V57" s="41"/>
+      <c r="W57" s="41"/>
+      <c r="X57" s="41"/>
+      <c r="Y57" s="41"/>
+      <c r="Z57" s="41"/>
+      <c r="AA57" s="41"/>
+      <c r="AB57" s="41"/>
+      <c r="AC57" s="41"/>
+      <c r="AD57" s="41"/>
+      <c r="AE57" s="41"/>
+      <c r="AF57" s="41"/>
+      <c r="AG57" s="41"/>
+      <c r="AH57" s="41"/>
+      <c r="AI57" s="41"/>
+      <c r="AJ57" s="41"/>
+      <c r="AK57" s="41"/>
+      <c r="AL57" s="41"/>
+      <c r="AM57" s="41"/>
+      <c r="AN57" s="41"/>
+      <c r="AO57" s="41"/>
+      <c r="AP57" s="41"/>
+      <c r="AQ57" s="41"/>
+      <c r="AR57" s="41"/>
+      <c r="AS57" s="41"/>
+      <c r="AT57" s="41"/>
+      <c r="AU57" s="41"/>
+      <c r="AV57" s="41"/>
+      <c r="AW57" s="41"/>
+      <c r="AX57" s="41"/>
+      <c r="AY57" s="41"/>
+      <c r="AZ57" s="41"/>
+      <c r="BA57" s="41"/>
+      <c r="BB57" s="41"/>
+      <c r="BC57" s="41"/>
+      <c r="BD57" s="41"/>
+      <c r="BE57" s="41"/>
+      <c r="BF57" s="41"/>
+      <c r="BG57" s="41"/>
+      <c r="BH57" s="41"/>
+      <c r="BI57" s="41"/>
+      <c r="BJ57" s="41"/>
+      <c r="BK57" s="41"/>
+      <c r="BL57" s="41"/>
+      <c r="BM57" s="41"/>
+      <c r="BN57" s="41"/>
+      <c r="BO57" s="41"/>
+      <c r="BP57" s="41"/>
+      <c r="BQ57" s="41"/>
+      <c r="BR57" s="41"/>
+      <c r="BS57" s="41"/>
+      <c r="BT57" s="41"/>
+      <c r="BU57" s="41"/>
+      <c r="BV57" s="41"/>
+      <c r="BW57" s="41"/>
+      <c r="BX57" s="41"/>
+      <c r="BY57" s="41"/>
+      <c r="BZ57" s="41"/>
+      <c r="CA57" s="41"/>
+      <c r="CB57" s="41"/>
+      <c r="CC57" s="41"/>
+      <c r="CD57" s="41"/>
+      <c r="CE57" s="41"/>
+      <c r="CF57" s="41"/>
+      <c r="CG57" s="41"/>
+      <c r="CH57" s="41"/>
+      <c r="CI57" s="41"/>
+      <c r="CJ57" s="41"/>
+      <c r="CK57" s="41"/>
+      <c r="CL57" s="41"/>
+      <c r="CM57" s="41"/>
+      <c r="CN57" s="41"/>
+      <c r="CO57" s="41"/>
+      <c r="CP57" s="41"/>
+      <c r="CQ57" s="41"/>
+      <c r="CR57" s="41"/>
+      <c r="CS57" s="41"/>
+      <c r="CT57" s="41"/>
+      <c r="CU57" s="41"/>
+      <c r="CV57" s="41"/>
+      <c r="CW57" s="41"/>
+      <c r="CX57" s="41"/>
+      <c r="CY57" s="41"/>
+      <c r="CZ57" s="41"/>
+      <c r="DA57" s="41"/>
+      <c r="DB57" s="41"/>
+    </row>
+    <row r="58" spans="2:106" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
+      <c r="K58" s="3"/>
+      <c r="L58" s="3"/>
+      <c r="M58" s="3"/>
+      <c r="N58" s="3"/>
+      <c r="O58" s="3"/>
+      <c r="P58" s="3"/>
+      <c r="Q58" s="3"/>
+      <c r="R58" s="3"/>
+      <c r="S58" s="3"/>
+      <c r="T58" s="3"/>
+      <c r="U58" s="3"/>
+      <c r="V58" s="3"/>
+      <c r="W58" s="3"/>
+      <c r="X58" s="3"/>
+      <c r="Y58" s="3"/>
+      <c r="Z58" s="3"/>
+      <c r="AA58" s="3"/>
+      <c r="AB58" s="3"/>
+      <c r="AC58" s="3"/>
+      <c r="AD58" s="3"/>
+      <c r="AE58" s="3"/>
+      <c r="AF58" s="3"/>
+      <c r="AG58" s="3"/>
+      <c r="AH58" s="3"/>
+      <c r="AI58" s="3"/>
+      <c r="AJ58" s="3"/>
+      <c r="AK58" s="3"/>
+      <c r="AL58" s="3"/>
+      <c r="AM58" s="3"/>
+      <c r="AN58" s="3"/>
+      <c r="AO58" s="3"/>
+      <c r="AP58" s="3"/>
+      <c r="AQ58" s="3"/>
+      <c r="AR58" s="3"/>
+      <c r="AS58" s="3"/>
+      <c r="AT58" s="3"/>
+      <c r="AU58" s="3"/>
+      <c r="AV58" s="3"/>
+      <c r="AW58" s="3"/>
+      <c r="AX58" s="3"/>
+      <c r="AY58" s="3"/>
+      <c r="AZ58" s="3"/>
+      <c r="BA58" s="3"/>
+      <c r="BB58" s="3"/>
+      <c r="BC58" s="3"/>
+      <c r="BD58" s="3"/>
+      <c r="BE58" s="3"/>
+      <c r="BF58" s="3"/>
+      <c r="BG58" s="3"/>
+      <c r="BH58" s="3"/>
+      <c r="BI58" s="3"/>
+      <c r="BJ58" s="3"/>
+      <c r="BK58" s="3"/>
+      <c r="BL58" s="3"/>
+      <c r="BM58" s="3"/>
+      <c r="BN58" s="3"/>
+      <c r="BO58" s="3"/>
+      <c r="BP58" s="3"/>
+      <c r="BQ58" s="3"/>
+      <c r="BR58" s="3"/>
+      <c r="BS58" s="3"/>
+      <c r="BT58" s="3"/>
+      <c r="BU58" s="3"/>
+      <c r="BV58" s="3"/>
+      <c r="BW58" s="3"/>
+      <c r="BX58" s="3"/>
+      <c r="BY58" s="3"/>
+      <c r="BZ58" s="3"/>
+      <c r="CA58" s="3"/>
+      <c r="CB58" s="3"/>
+      <c r="CC58" s="3"/>
+      <c r="CD58" s="3"/>
+      <c r="CE58" s="3"/>
+      <c r="CF58" s="3"/>
+      <c r="CG58" s="3"/>
+      <c r="CH58" s="3"/>
+      <c r="CI58" s="3"/>
+      <c r="CJ58" s="3"/>
+      <c r="CK58" s="3"/>
+      <c r="CL58" s="3"/>
+      <c r="CM58" s="3"/>
+      <c r="CN58" s="3"/>
+      <c r="CO58" s="3"/>
+      <c r="CP58" s="3"/>
+      <c r="CQ58" s="3"/>
+      <c r="CR58" s="3"/>
+      <c r="CS58" s="3"/>
+      <c r="CT58" s="3"/>
+      <c r="CU58" s="3"/>
+      <c r="CV58" s="3"/>
+      <c r="CW58" s="3"/>
+      <c r="CX58" s="3"/>
+      <c r="CY58" s="3"/>
+      <c r="CZ58" s="3"/>
+      <c r="DA58" s="3"/>
+      <c r="DB58" s="3"/>
+    </row>
+    <row r="59" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3"/>
+      <c r="J59" s="3"/>
+      <c r="K59" s="3"/>
+      <c r="L59" s="3"/>
+      <c r="M59" s="3"/>
+      <c r="N59" s="3"/>
+      <c r="O59" s="3"/>
+      <c r="P59" s="3"/>
+      <c r="Q59" s="3"/>
+      <c r="R59" s="3"/>
+      <c r="S59" s="3"/>
+      <c r="T59" s="3"/>
+      <c r="U59" s="3"/>
+      <c r="V59" s="3"/>
+      <c r="W59" s="3"/>
+      <c r="X59" s="3"/>
+      <c r="Y59" s="3"/>
+      <c r="Z59" s="3"/>
+      <c r="AA59" s="3"/>
+      <c r="AB59" s="3"/>
+      <c r="AC59" s="3"/>
+      <c r="AD59" s="3"/>
+      <c r="AE59" s="3"/>
+      <c r="AF59" s="3"/>
+      <c r="AG59" s="3"/>
+      <c r="AH59" s="3"/>
+      <c r="AI59" s="3"/>
+      <c r="AJ59" s="3"/>
+      <c r="AK59" s="3"/>
+      <c r="AL59" s="3"/>
+      <c r="AM59" s="3"/>
+      <c r="AN59" s="3"/>
+      <c r="AO59" s="3"/>
+      <c r="AP59" s="3"/>
+      <c r="AQ59" s="3"/>
+      <c r="AR59" s="3"/>
+      <c r="AS59" s="3"/>
+      <c r="AT59" s="3"/>
+      <c r="AU59" s="3"/>
+      <c r="AV59" s="3"/>
+      <c r="AW59" s="3"/>
+      <c r="AX59" s="3"/>
+      <c r="AY59" s="3"/>
+      <c r="AZ59" s="3"/>
+      <c r="BA59" s="3"/>
+      <c r="BB59" s="3"/>
+      <c r="BC59" s="3"/>
+      <c r="BD59" s="3"/>
+      <c r="BE59" s="3"/>
+      <c r="BF59" s="3"/>
+      <c r="BG59" s="3"/>
+      <c r="BH59" s="3"/>
+      <c r="BI59" s="3"/>
+      <c r="BJ59" s="3"/>
+      <c r="BK59" s="3"/>
+      <c r="BL59" s="3"/>
+      <c r="BM59" s="3"/>
+      <c r="BN59" s="3"/>
+      <c r="BO59" s="3"/>
+      <c r="BP59" s="3"/>
+      <c r="BQ59" s="3"/>
+      <c r="BR59" s="3"/>
+      <c r="BS59" s="3"/>
+      <c r="BT59" s="3"/>
+      <c r="BU59" s="3"/>
+      <c r="BV59" s="3"/>
+      <c r="BW59" s="3"/>
+      <c r="BX59" s="3"/>
+      <c r="BY59" s="3"/>
+      <c r="BZ59" s="3"/>
+      <c r="CA59" s="3"/>
+      <c r="CB59" s="3"/>
+      <c r="CC59" s="3"/>
+      <c r="CD59" s="3"/>
+      <c r="CE59" s="3"/>
+      <c r="CF59" s="3"/>
+      <c r="CG59" s="3"/>
+      <c r="CH59" s="3"/>
+      <c r="CI59" s="3"/>
+      <c r="CJ59" s="3"/>
+      <c r="CK59" s="3"/>
+      <c r="CL59" s="3"/>
+      <c r="CM59" s="3"/>
+      <c r="CN59" s="3"/>
+      <c r="CO59" s="3"/>
+      <c r="CP59" s="3"/>
+      <c r="CQ59" s="3"/>
+      <c r="CR59" s="3"/>
+      <c r="CS59" s="3"/>
+      <c r="CT59" s="3"/>
+      <c r="CU59" s="3"/>
+      <c r="CV59" s="3"/>
+      <c r="CW59" s="3"/>
+      <c r="CX59" s="3"/>
+      <c r="CY59" s="3"/>
+      <c r="CZ59" s="3"/>
+      <c r="DA59" s="3"/>
+      <c r="DB59" s="3"/>
+    </row>
+    <row r="60" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B60" s="78"/>
+      <c r="C60" s="73"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="65"/>
+      <c r="F60" s="65"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="14" t="str">
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
-      <c r="I54" s="43"/>
-      <c r="J54" s="43"/>
-      <c r="K54" s="43"/>
-      <c r="L54" s="43"/>
-      <c r="M54" s="43"/>
-      <c r="N54" s="43"/>
-      <c r="O54" s="43"/>
-      <c r="P54" s="43"/>
-      <c r="Q54" s="43"/>
-      <c r="R54" s="43"/>
-      <c r="S54" s="43"/>
-      <c r="T54" s="43"/>
-      <c r="U54" s="43"/>
-      <c r="V54" s="43"/>
-      <c r="W54" s="43"/>
-      <c r="X54" s="43"/>
-      <c r="Y54" s="43"/>
-      <c r="Z54" s="43"/>
-      <c r="AA54" s="43"/>
-      <c r="AB54" s="43"/>
-      <c r="AC54" s="43"/>
-      <c r="AD54" s="43"/>
-      <c r="AE54" s="43"/>
-      <c r="AF54" s="43"/>
-      <c r="AG54" s="43"/>
-      <c r="AH54" s="43"/>
-      <c r="AI54" s="43"/>
-      <c r="AJ54" s="43"/>
-      <c r="AK54" s="43"/>
-      <c r="AL54" s="43"/>
-      <c r="AM54" s="43"/>
-      <c r="AN54" s="43"/>
-      <c r="AO54" s="43"/>
-      <c r="AP54" s="43"/>
-      <c r="AQ54" s="43"/>
-      <c r="AR54" s="43"/>
-      <c r="AS54" s="43"/>
-      <c r="AT54" s="43"/>
-      <c r="AU54" s="43"/>
-      <c r="AV54" s="43"/>
-      <c r="AW54" s="43"/>
-      <c r="AX54" s="43"/>
-      <c r="AY54" s="43"/>
-      <c r="AZ54" s="43"/>
-      <c r="BA54" s="43"/>
-      <c r="BB54" s="43"/>
-      <c r="BC54" s="43"/>
-      <c r="BD54" s="43"/>
-      <c r="BE54" s="43"/>
-      <c r="BF54" s="43"/>
-      <c r="BG54" s="43"/>
-      <c r="BH54" s="43"/>
-      <c r="BI54" s="43"/>
-      <c r="BJ54" s="43"/>
-      <c r="BK54" s="43"/>
-      <c r="BL54" s="43"/>
-      <c r="BM54" s="43"/>
-      <c r="BN54" s="43"/>
-      <c r="BO54" s="43"/>
-      <c r="BP54" s="43"/>
-      <c r="BQ54" s="43"/>
-      <c r="BR54" s="43"/>
-      <c r="BS54" s="43"/>
-      <c r="BT54" s="43"/>
-      <c r="BU54" s="43"/>
-      <c r="BV54" s="43"/>
-      <c r="BW54" s="43"/>
-      <c r="BX54" s="43"/>
-      <c r="BY54" s="43"/>
-      <c r="BZ54" s="43"/>
-      <c r="CA54" s="43"/>
-      <c r="CB54" s="43"/>
-      <c r="CC54" s="43"/>
-      <c r="CD54" s="43"/>
-      <c r="CE54" s="43"/>
-      <c r="CF54" s="43"/>
-      <c r="CG54" s="43"/>
-      <c r="CH54" s="43"/>
-      <c r="CI54" s="43"/>
-      <c r="CJ54" s="43"/>
-      <c r="CK54" s="43"/>
-      <c r="CL54" s="43"/>
-      <c r="CM54" s="43"/>
-      <c r="CN54" s="43"/>
-      <c r="CO54" s="43"/>
-      <c r="CP54" s="43"/>
-      <c r="CQ54" s="43"/>
-      <c r="CR54" s="43"/>
-      <c r="CS54" s="43"/>
-      <c r="CT54" s="43"/>
-      <c r="CU54" s="43"/>
-      <c r="CV54" s="43"/>
-      <c r="CW54" s="43"/>
-      <c r="CX54" s="43"/>
-      <c r="CY54" s="43"/>
-      <c r="CZ54" s="43"/>
-      <c r="DA54" s="43"/>
-      <c r="DB54" s="43"/>
+      <c r="I60" s="41"/>
+      <c r="J60" s="41"/>
+      <c r="K60" s="41"/>
+      <c r="L60" s="41"/>
+      <c r="M60" s="41"/>
+      <c r="N60" s="41"/>
+      <c r="O60" s="41"/>
+      <c r="P60" s="41"/>
+      <c r="Q60" s="41"/>
+      <c r="R60" s="41"/>
+      <c r="S60" s="41"/>
+      <c r="T60" s="41"/>
+      <c r="U60" s="41"/>
+      <c r="V60" s="41"/>
+      <c r="W60" s="41"/>
+      <c r="X60" s="41"/>
+      <c r="Y60" s="41"/>
+      <c r="Z60" s="41"/>
+      <c r="AA60" s="41"/>
+      <c r="AB60" s="41"/>
+      <c r="AC60" s="41"/>
+      <c r="AD60" s="41"/>
+      <c r="AE60" s="41"/>
+      <c r="AF60" s="41"/>
+      <c r="AG60" s="41"/>
+      <c r="AH60" s="41"/>
+      <c r="AI60" s="41"/>
+      <c r="AJ60" s="41"/>
+      <c r="AK60" s="41"/>
+      <c r="AL60" s="41"/>
+      <c r="AM60" s="41"/>
+      <c r="AN60" s="41"/>
+      <c r="AO60" s="41"/>
+      <c r="AP60" s="41"/>
+      <c r="AQ60" s="41"/>
+      <c r="AR60" s="41"/>
+      <c r="AS60" s="41"/>
+      <c r="AT60" s="41"/>
+      <c r="AU60" s="41"/>
+      <c r="AV60" s="41"/>
+      <c r="AW60" s="41"/>
+      <c r="AX60" s="41"/>
+      <c r="AY60" s="41"/>
+      <c r="AZ60" s="41"/>
+      <c r="BA60" s="41"/>
+      <c r="BB60" s="41"/>
+      <c r="BC60" s="41"/>
+      <c r="BD60" s="41"/>
+      <c r="BE60" s="41"/>
+      <c r="BF60" s="41"/>
+      <c r="BG60" s="41"/>
+      <c r="BH60" s="41"/>
+      <c r="BI60" s="41"/>
+      <c r="BJ60" s="41"/>
+      <c r="BK60" s="41"/>
+      <c r="BL60" s="41"/>
+      <c r="BM60" s="41"/>
+      <c r="BN60" s="41"/>
+      <c r="BO60" s="41"/>
+      <c r="BP60" s="41"/>
+      <c r="BQ60" s="41"/>
+      <c r="BR60" s="41"/>
+      <c r="BS60" s="41"/>
+      <c r="BT60" s="41"/>
+      <c r="BU60" s="41"/>
+      <c r="BV60" s="41"/>
+      <c r="BW60" s="41"/>
+      <c r="BX60" s="41"/>
+      <c r="BY60" s="41"/>
+      <c r="BZ60" s="41"/>
+      <c r="CA60" s="41"/>
+      <c r="CB60" s="41"/>
+      <c r="CC60" s="41"/>
+      <c r="CD60" s="41"/>
+      <c r="CE60" s="41"/>
+      <c r="CF60" s="41"/>
+      <c r="CG60" s="41"/>
+      <c r="CH60" s="41"/>
+      <c r="CI60" s="41"/>
+      <c r="CJ60" s="41"/>
+      <c r="CK60" s="41"/>
+      <c r="CL60" s="41"/>
+      <c r="CM60" s="41"/>
+      <c r="CN60" s="41"/>
+      <c r="CO60" s="41"/>
+      <c r="CP60" s="41"/>
+      <c r="CQ60" s="41"/>
+      <c r="CR60" s="41"/>
+      <c r="CS60" s="41"/>
+      <c r="CT60" s="41"/>
+      <c r="CU60" s="41"/>
+      <c r="CV60" s="41"/>
+      <c r="CW60" s="41"/>
+      <c r="CX60" s="41"/>
+      <c r="CY60" s="41"/>
+      <c r="CZ60" s="41"/>
+      <c r="DA60" s="41"/>
+      <c r="DB60" s="41"/>
+    </row>
+    <row r="61" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B61" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C61" s="36"/>
+      <c r="D61" s="37"/>
+      <c r="E61" s="38"/>
+      <c r="F61" s="39"/>
+      <c r="G61" s="40"/>
+      <c r="H61" s="40" t="str">
+        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <v/>
+      </c>
+      <c r="I61" s="43"/>
+      <c r="J61" s="43"/>
+      <c r="K61" s="43"/>
+      <c r="L61" s="43"/>
+      <c r="M61" s="43"/>
+      <c r="N61" s="43"/>
+      <c r="O61" s="43"/>
+      <c r="P61" s="43"/>
+      <c r="Q61" s="43"/>
+      <c r="R61" s="43"/>
+      <c r="S61" s="43"/>
+      <c r="T61" s="43"/>
+      <c r="U61" s="43"/>
+      <c r="V61" s="43"/>
+      <c r="W61" s="43"/>
+      <c r="X61" s="43"/>
+      <c r="Y61" s="43"/>
+      <c r="Z61" s="43"/>
+      <c r="AA61" s="43"/>
+      <c r="AB61" s="43"/>
+      <c r="AC61" s="43"/>
+      <c r="AD61" s="43"/>
+      <c r="AE61" s="43"/>
+      <c r="AF61" s="43"/>
+      <c r="AG61" s="43"/>
+      <c r="AH61" s="43"/>
+      <c r="AI61" s="43"/>
+      <c r="AJ61" s="43"/>
+      <c r="AK61" s="43"/>
+      <c r="AL61" s="43"/>
+      <c r="AM61" s="43"/>
+      <c r="AN61" s="43"/>
+      <c r="AO61" s="43"/>
+      <c r="AP61" s="43"/>
+      <c r="AQ61" s="43"/>
+      <c r="AR61" s="43"/>
+      <c r="AS61" s="43"/>
+      <c r="AT61" s="43"/>
+      <c r="AU61" s="43"/>
+      <c r="AV61" s="43"/>
+      <c r="AW61" s="43"/>
+      <c r="AX61" s="43"/>
+      <c r="AY61" s="43"/>
+      <c r="AZ61" s="43"/>
+      <c r="BA61" s="43"/>
+      <c r="BB61" s="43"/>
+      <c r="BC61" s="43"/>
+      <c r="BD61" s="43"/>
+      <c r="BE61" s="43"/>
+      <c r="BF61" s="43"/>
+      <c r="BG61" s="43"/>
+      <c r="BH61" s="43"/>
+      <c r="BI61" s="43"/>
+      <c r="BJ61" s="43"/>
+      <c r="BK61" s="43"/>
+      <c r="BL61" s="43"/>
+      <c r="BM61" s="43"/>
+      <c r="BN61" s="43"/>
+      <c r="BO61" s="43"/>
+      <c r="BP61" s="43"/>
+      <c r="BQ61" s="43"/>
+      <c r="BR61" s="43"/>
+      <c r="BS61" s="43"/>
+      <c r="BT61" s="43"/>
+      <c r="BU61" s="43"/>
+      <c r="BV61" s="43"/>
+      <c r="BW61" s="43"/>
+      <c r="BX61" s="43"/>
+      <c r="BY61" s="43"/>
+      <c r="BZ61" s="43"/>
+      <c r="CA61" s="43"/>
+      <c r="CB61" s="43"/>
+      <c r="CC61" s="43"/>
+      <c r="CD61" s="43"/>
+      <c r="CE61" s="43"/>
+      <c r="CF61" s="43"/>
+      <c r="CG61" s="43"/>
+      <c r="CH61" s="43"/>
+      <c r="CI61" s="43"/>
+      <c r="CJ61" s="43"/>
+      <c r="CK61" s="43"/>
+      <c r="CL61" s="43"/>
+      <c r="CM61" s="43"/>
+      <c r="CN61" s="43"/>
+      <c r="CO61" s="43"/>
+      <c r="CP61" s="43"/>
+      <c r="CQ61" s="43"/>
+      <c r="CR61" s="43"/>
+      <c r="CS61" s="43"/>
+      <c r="CT61" s="43"/>
+      <c r="CU61" s="43"/>
+      <c r="CV61" s="43"/>
+      <c r="CW61" s="43"/>
+      <c r="CX61" s="43"/>
+      <c r="CY61" s="43"/>
+      <c r="CZ61" s="43"/>
+      <c r="DA61" s="43"/>
+      <c r="DB61" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="17">
@@ -8684,7 +9502,7 @@
     <mergeCell ref="BT4:BZ4"/>
     <mergeCell ref="CA4:CG4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D53:D54 D7:D50">
+  <conditionalFormatting sqref="D60:D61 D7:D57">
     <cfRule type="dataBar" priority="53">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8698,12 +9516,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I53:BL54 I29:DB50">
+  <conditionalFormatting sqref="I60:BL61 I29:DB57">
     <cfRule type="expression" dxfId="44" priority="72">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I53:BL54 I29:DB50">
+  <conditionalFormatting sqref="I60:BL61 I29:DB57">
     <cfRule type="expression" dxfId="43" priority="66">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -8789,12 +9607,12 @@
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM53:CG54">
+  <conditionalFormatting sqref="BM60:CG61">
     <cfRule type="expression" dxfId="23" priority="21">
       <formula>AND(TODAY()&gt;=BM$5,TODAY()&lt;BN$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM53:CG54">
+  <conditionalFormatting sqref="BM60:CG61">
     <cfRule type="expression" dxfId="22" priority="19">
       <formula>AND(task_start&lt;=BM$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BM$5)</formula>
     </cfRule>
@@ -8841,12 +9659,12 @@
       <formula>AND(task_end&gt;=BM$5,task_start&lt;BN$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CH53:DB54">
+  <conditionalFormatting sqref="CH60:DB61">
     <cfRule type="expression" dxfId="11" priority="9">
       <formula>AND(TODAY()&gt;=CH$5,TODAY()&lt;CI$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CH53:DB54">
+  <conditionalFormatting sqref="CH60:DB61">
     <cfRule type="expression" dxfId="10" priority="7">
       <formula>AND(task_start&lt;=CH$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CH$5)</formula>
     </cfRule>
@@ -8899,8 +9717,8 @@
     </dataValidation>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="37" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.35433070866141736" right="0.35433070866141736" top="0.35433070866141736" bottom="0.51181102362204722" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="8" scale="57" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter differentFirst="1" scaleWithDoc="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
@@ -8920,7 +9738,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D53:D54 D7:D50</xm:sqref>
+          <xm:sqref>D60:D61 D7:D57</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -8943,79 +9761,79 @@
     <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:2" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="46" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="46"/>
     </row>
     <row r="3" spans="1:2" s="51" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="82" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="52"/>
     </row>
     <row r="4" spans="1:2" s="48" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A4" s="49" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="50" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="49" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="45" customFormat="1" ht="205.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="54" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="48" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A8" s="49" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="50" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="45" customFormat="1" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="53" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="48" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A11" s="49" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="50" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="45" customFormat="1" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="53" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="48" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A14" s="49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="50" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="50" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Leaderboard and Scene switching
I added a random scoring for the leaderboard as well as made it possible to switch from the login/register scene to the start scene and from the leaderboard back to the start scene.
</commit_message>
<xml_diff>
--- a/Rampage/Rampage Gantt Chart.xlsx
+++ b/Rampage/Rampage Gantt Chart.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCA815E-57D1-4D3D-9719-4DC39268090A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B29C99-62C7-44FD-B6A3-FE4DADCC1107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11304" yWindow="0" windowWidth="11640" windowHeight="10824" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="83">
   <si>
     <t>Create a Project Schedule in this worksheet.
 Enter title of this project in cell B1. 
@@ -127,12 +127,6 @@
 Continue entering tasks in cells A10 through A13 or go to cell A14 to learn more.</t>
   </si>
   <si>
-    <t>Task 4</t>
-  </si>
-  <si>
-    <t>Task 5</t>
-  </si>
-  <si>
     <t>The cell at right contains the Phase 2 sample title. 
 You can create a new phase at any time within column B. This project schedule does not require phases. To remove the phase, simply delete the row.
 To create a new phase block in this row, enter a new Title in cell at right.
@@ -152,16 +146,7 @@
     <t>Sprint 3</t>
   </si>
   <si>
-    <t>Task 2</t>
-  </si>
-  <si>
-    <t>Task 3</t>
-  </si>
-  <si>
     <t>Sprint 4</t>
-  </si>
-  <si>
-    <t>date</t>
   </si>
   <si>
     <t>Insert new rows ABOVE this one</t>
@@ -325,9 +310,6 @@
     <t>HUD Functionality</t>
   </si>
   <si>
-    <t>Menus</t>
-  </si>
-  <si>
     <t xml:space="preserve">Character Functionality </t>
   </si>
   <si>
@@ -335,6 +317,18 @@
   </si>
   <si>
     <t>NPCS/ Building, Main Playing Scene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technical Document </t>
+  </si>
+  <si>
+    <t>Tameka, Andrea, Shikha</t>
+  </si>
+  <si>
+    <t>Menus, Audio</t>
   </si>
 </sst>
 </file>
@@ -997,6 +991,12 @@
     <xf numFmtId="165" fontId="0" fillId="10" borderId="2" xfId="10" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1008,12 +1008,6 @@
     </xf>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1998,14 +1992,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1">
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:DB61"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:DB63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" view="pageBreakPreview" zoomScale="59" zoomScaleNormal="110" zoomScaleSheetLayoutView="59" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B53" sqref="B53"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="60" zoomScaleNormal="60" zoomScaleSheetLayoutView="59" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AP31" sqref="AP31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2044,7 +2036,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="58" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -2065,166 +2057,166 @@
         <v>2</v>
       </c>
       <c r="B3" s="60"/>
-      <c r="C3" s="93" t="s">
+      <c r="C3" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="94"/>
-      <c r="E3" s="92">
+      <c r="D3" s="90"/>
+      <c r="E3" s="94">
         <v>45159</v>
       </c>
-      <c r="F3" s="92"/>
+      <c r="F3" s="94"/>
     </row>
     <row r="4" spans="1:106" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="93" t="s">
+      <c r="C4" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="94"/>
+      <c r="D4" s="90"/>
       <c r="E4" s="6">
-        <v>1</v>
-      </c>
-      <c r="I4" s="89">
+        <v>10</v>
+      </c>
+      <c r="I4" s="91">
         <f>I5</f>
-        <v>45159</v>
-      </c>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="90"/>
-      <c r="N4" s="90"/>
-      <c r="O4" s="91"/>
-      <c r="P4" s="89">
+        <v>45222</v>
+      </c>
+      <c r="J4" s="92"/>
+      <c r="K4" s="92"/>
+      <c r="L4" s="92"/>
+      <c r="M4" s="92"/>
+      <c r="N4" s="92"/>
+      <c r="O4" s="93"/>
+      <c r="P4" s="91">
         <f>P5</f>
-        <v>45166</v>
-      </c>
-      <c r="Q4" s="90"/>
-      <c r="R4" s="90"/>
-      <c r="S4" s="90"/>
-      <c r="T4" s="90"/>
-      <c r="U4" s="90"/>
-      <c r="V4" s="91"/>
-      <c r="W4" s="89">
+        <v>45229</v>
+      </c>
+      <c r="Q4" s="92"/>
+      <c r="R4" s="92"/>
+      <c r="S4" s="92"/>
+      <c r="T4" s="92"/>
+      <c r="U4" s="92"/>
+      <c r="V4" s="93"/>
+      <c r="W4" s="91">
         <f>W5</f>
-        <v>45173</v>
-      </c>
-      <c r="X4" s="90"/>
-      <c r="Y4" s="90"/>
-      <c r="Z4" s="90"/>
-      <c r="AA4" s="90"/>
-      <c r="AB4" s="90"/>
-      <c r="AC4" s="91"/>
-      <c r="AD4" s="89">
+        <v>45236</v>
+      </c>
+      <c r="X4" s="92"/>
+      <c r="Y4" s="92"/>
+      <c r="Z4" s="92"/>
+      <c r="AA4" s="92"/>
+      <c r="AB4" s="92"/>
+      <c r="AC4" s="93"/>
+      <c r="AD4" s="91">
         <f>AD5</f>
-        <v>45180</v>
-      </c>
-      <c r="AE4" s="90"/>
-      <c r="AF4" s="90"/>
-      <c r="AG4" s="90"/>
-      <c r="AH4" s="90"/>
-      <c r="AI4" s="90"/>
-      <c r="AJ4" s="91"/>
-      <c r="AK4" s="89">
+        <v>45243</v>
+      </c>
+      <c r="AE4" s="92"/>
+      <c r="AF4" s="92"/>
+      <c r="AG4" s="92"/>
+      <c r="AH4" s="92"/>
+      <c r="AI4" s="92"/>
+      <c r="AJ4" s="93"/>
+      <c r="AK4" s="91">
         <f>AK5</f>
-        <v>45187</v>
-      </c>
-      <c r="AL4" s="90"/>
-      <c r="AM4" s="90"/>
-      <c r="AN4" s="90"/>
-      <c r="AO4" s="90"/>
-      <c r="AP4" s="90"/>
-      <c r="AQ4" s="91"/>
-      <c r="AR4" s="89">
+        <v>45250</v>
+      </c>
+      <c r="AL4" s="92"/>
+      <c r="AM4" s="92"/>
+      <c r="AN4" s="92"/>
+      <c r="AO4" s="92"/>
+      <c r="AP4" s="92"/>
+      <c r="AQ4" s="93"/>
+      <c r="AR4" s="91">
         <f>AR5</f>
-        <v>45194</v>
-      </c>
-      <c r="AS4" s="90"/>
-      <c r="AT4" s="90"/>
-      <c r="AU4" s="90"/>
-      <c r="AV4" s="90"/>
-      <c r="AW4" s="90"/>
-      <c r="AX4" s="91"/>
-      <c r="AY4" s="89">
+        <v>45257</v>
+      </c>
+      <c r="AS4" s="92"/>
+      <c r="AT4" s="92"/>
+      <c r="AU4" s="92"/>
+      <c r="AV4" s="92"/>
+      <c r="AW4" s="92"/>
+      <c r="AX4" s="93"/>
+      <c r="AY4" s="91">
         <f>AY5</f>
-        <v>45201</v>
-      </c>
-      <c r="AZ4" s="90"/>
-      <c r="BA4" s="90"/>
-      <c r="BB4" s="90"/>
-      <c r="BC4" s="90"/>
-      <c r="BD4" s="90"/>
-      <c r="BE4" s="91"/>
-      <c r="BF4" s="89">
+        <v>45264</v>
+      </c>
+      <c r="AZ4" s="92"/>
+      <c r="BA4" s="92"/>
+      <c r="BB4" s="92"/>
+      <c r="BC4" s="92"/>
+      <c r="BD4" s="92"/>
+      <c r="BE4" s="93"/>
+      <c r="BF4" s="91">
         <f>BF5</f>
-        <v>45208</v>
-      </c>
-      <c r="BG4" s="90"/>
-      <c r="BH4" s="90"/>
-      <c r="BI4" s="90"/>
-      <c r="BJ4" s="90"/>
-      <c r="BK4" s="90"/>
-      <c r="BL4" s="91"/>
-      <c r="BM4" s="89">
+        <v>45271</v>
+      </c>
+      <c r="BG4" s="92"/>
+      <c r="BH4" s="92"/>
+      <c r="BI4" s="92"/>
+      <c r="BJ4" s="92"/>
+      <c r="BK4" s="92"/>
+      <c r="BL4" s="93"/>
+      <c r="BM4" s="91">
         <f>BM5</f>
-        <v>45215</v>
-      </c>
-      <c r="BN4" s="90"/>
-      <c r="BO4" s="90"/>
-      <c r="BP4" s="90"/>
-      <c r="BQ4" s="90"/>
-      <c r="BR4" s="90"/>
-      <c r="BS4" s="91"/>
-      <c r="BT4" s="89">
+        <v>45278</v>
+      </c>
+      <c r="BN4" s="92"/>
+      <c r="BO4" s="92"/>
+      <c r="BP4" s="92"/>
+      <c r="BQ4" s="92"/>
+      <c r="BR4" s="92"/>
+      <c r="BS4" s="93"/>
+      <c r="BT4" s="91">
         <f>BT5</f>
-        <v>45222</v>
-      </c>
-      <c r="BU4" s="90"/>
-      <c r="BV4" s="90"/>
-      <c r="BW4" s="90"/>
-      <c r="BX4" s="90"/>
-      <c r="BY4" s="90"/>
-      <c r="BZ4" s="91"/>
-      <c r="CA4" s="89">
+        <v>45285</v>
+      </c>
+      <c r="BU4" s="92"/>
+      <c r="BV4" s="92"/>
+      <c r="BW4" s="92"/>
+      <c r="BX4" s="92"/>
+      <c r="BY4" s="92"/>
+      <c r="BZ4" s="93"/>
+      <c r="CA4" s="91">
         <f>CA5</f>
-        <v>45229</v>
-      </c>
-      <c r="CB4" s="90"/>
-      <c r="CC4" s="90"/>
-      <c r="CD4" s="90"/>
-      <c r="CE4" s="90"/>
-      <c r="CF4" s="90"/>
-      <c r="CG4" s="91"/>
-      <c r="CH4" s="89">
+        <v>45292</v>
+      </c>
+      <c r="CB4" s="92"/>
+      <c r="CC4" s="92"/>
+      <c r="CD4" s="92"/>
+      <c r="CE4" s="92"/>
+      <c r="CF4" s="92"/>
+      <c r="CG4" s="93"/>
+      <c r="CH4" s="91">
         <f>CH5</f>
-        <v>45236</v>
-      </c>
-      <c r="CI4" s="90"/>
-      <c r="CJ4" s="90"/>
-      <c r="CK4" s="90"/>
-      <c r="CL4" s="90"/>
-      <c r="CM4" s="90"/>
-      <c r="CN4" s="91"/>
-      <c r="CO4" s="89">
+        <v>45299</v>
+      </c>
+      <c r="CI4" s="92"/>
+      <c r="CJ4" s="92"/>
+      <c r="CK4" s="92"/>
+      <c r="CL4" s="92"/>
+      <c r="CM4" s="92"/>
+      <c r="CN4" s="93"/>
+      <c r="CO4" s="91">
         <f>CO5</f>
-        <v>45243</v>
-      </c>
-      <c r="CP4" s="90"/>
-      <c r="CQ4" s="90"/>
-      <c r="CR4" s="90"/>
-      <c r="CS4" s="90"/>
-      <c r="CT4" s="90"/>
-      <c r="CU4" s="91"/>
-      <c r="CV4" s="89">
+        <v>45306</v>
+      </c>
+      <c r="CP4" s="92"/>
+      <c r="CQ4" s="92"/>
+      <c r="CR4" s="92"/>
+      <c r="CS4" s="92"/>
+      <c r="CT4" s="92"/>
+      <c r="CU4" s="93"/>
+      <c r="CV4" s="91">
         <f>CV5</f>
-        <v>45250</v>
-      </c>
-      <c r="CW4" s="90"/>
-      <c r="CX4" s="90"/>
-      <c r="CY4" s="90"/>
-      <c r="CZ4" s="90"/>
-      <c r="DA4" s="90"/>
-      <c r="DB4" s="91"/>
+        <v>45313</v>
+      </c>
+      <c r="CW4" s="92"/>
+      <c r="CX4" s="92"/>
+      <c r="CY4" s="92"/>
+      <c r="CZ4" s="92"/>
+      <c r="DA4" s="92"/>
+      <c r="DB4" s="93"/>
     </row>
     <row r="5" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="56" t="s">
@@ -2238,395 +2230,395 @@
       <c r="G5" s="79"/>
       <c r="I5" s="10">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>45159</v>
+        <v>45222</v>
       </c>
       <c r="J5" s="9">
         <f>I5+1</f>
-        <v>45160</v>
+        <v>45223</v>
       </c>
       <c r="K5" s="9">
         <f t="shared" ref="K5:AX5" si="0">J5+1</f>
-        <v>45161</v>
+        <v>45224</v>
       </c>
       <c r="L5" s="9">
         <f t="shared" si="0"/>
-        <v>45162</v>
+        <v>45225</v>
       </c>
       <c r="M5" s="9">
         <f t="shared" si="0"/>
-        <v>45163</v>
+        <v>45226</v>
       </c>
       <c r="N5" s="9">
         <f t="shared" si="0"/>
-        <v>45164</v>
+        <v>45227</v>
       </c>
       <c r="O5" s="11">
         <f t="shared" si="0"/>
-        <v>45165</v>
+        <v>45228</v>
       </c>
       <c r="P5" s="10">
         <f>O5+1</f>
-        <v>45166</v>
+        <v>45229</v>
       </c>
       <c r="Q5" s="9">
         <f>P5+1</f>
-        <v>45167</v>
+        <v>45230</v>
       </c>
       <c r="R5" s="9">
         <f t="shared" si="0"/>
-        <v>45168</v>
+        <v>45231</v>
       </c>
       <c r="S5" s="9">
         <f t="shared" si="0"/>
-        <v>45169</v>
+        <v>45232</v>
       </c>
       <c r="T5" s="9">
         <f t="shared" si="0"/>
-        <v>45170</v>
+        <v>45233</v>
       </c>
       <c r="U5" s="9">
         <f t="shared" si="0"/>
-        <v>45171</v>
+        <v>45234</v>
       </c>
       <c r="V5" s="11">
         <f t="shared" si="0"/>
-        <v>45172</v>
+        <v>45235</v>
       </c>
       <c r="W5" s="10">
         <f>V5+1</f>
-        <v>45173</v>
+        <v>45236</v>
       </c>
       <c r="X5" s="9">
         <f>W5+1</f>
-        <v>45174</v>
+        <v>45237</v>
       </c>
       <c r="Y5" s="9">
         <f t="shared" si="0"/>
-        <v>45175</v>
+        <v>45238</v>
       </c>
       <c r="Z5" s="9">
         <f t="shared" si="0"/>
-        <v>45176</v>
+        <v>45239</v>
       </c>
       <c r="AA5" s="9">
         <f t="shared" si="0"/>
-        <v>45177</v>
+        <v>45240</v>
       </c>
       <c r="AB5" s="9">
         <f t="shared" si="0"/>
-        <v>45178</v>
+        <v>45241</v>
       </c>
       <c r="AC5" s="11">
         <f t="shared" si="0"/>
-        <v>45179</v>
+        <v>45242</v>
       </c>
       <c r="AD5" s="10">
         <f>AC5+1</f>
-        <v>45180</v>
+        <v>45243</v>
       </c>
       <c r="AE5" s="9">
         <f>AD5+1</f>
-        <v>45181</v>
+        <v>45244</v>
       </c>
       <c r="AF5" s="9">
         <f t="shared" si="0"/>
-        <v>45182</v>
+        <v>45245</v>
       </c>
       <c r="AG5" s="9">
         <f t="shared" si="0"/>
-        <v>45183</v>
+        <v>45246</v>
       </c>
       <c r="AH5" s="9">
         <f t="shared" si="0"/>
-        <v>45184</v>
+        <v>45247</v>
       </c>
       <c r="AI5" s="9">
         <f t="shared" si="0"/>
-        <v>45185</v>
+        <v>45248</v>
       </c>
       <c r="AJ5" s="11">
         <f t="shared" si="0"/>
-        <v>45186</v>
+        <v>45249</v>
       </c>
       <c r="AK5" s="10">
         <f>AJ5+1</f>
-        <v>45187</v>
+        <v>45250</v>
       </c>
       <c r="AL5" s="9">
         <f>AK5+1</f>
-        <v>45188</v>
+        <v>45251</v>
       </c>
       <c r="AM5" s="9">
         <f t="shared" si="0"/>
-        <v>45189</v>
+        <v>45252</v>
       </c>
       <c r="AN5" s="9">
         <f t="shared" si="0"/>
-        <v>45190</v>
+        <v>45253</v>
       </c>
       <c r="AO5" s="9">
         <f t="shared" si="0"/>
-        <v>45191</v>
+        <v>45254</v>
       </c>
       <c r="AP5" s="9">
         <f t="shared" si="0"/>
-        <v>45192</v>
+        <v>45255</v>
       </c>
       <c r="AQ5" s="11">
         <f t="shared" si="0"/>
-        <v>45193</v>
+        <v>45256</v>
       </c>
       <c r="AR5" s="10">
         <f>AQ5+1</f>
-        <v>45194</v>
+        <v>45257</v>
       </c>
       <c r="AS5" s="9">
         <f>AR5+1</f>
-        <v>45195</v>
+        <v>45258</v>
       </c>
       <c r="AT5" s="9">
         <f t="shared" si="0"/>
-        <v>45196</v>
+        <v>45259</v>
       </c>
       <c r="AU5" s="9">
         <f t="shared" si="0"/>
-        <v>45197</v>
+        <v>45260</v>
       </c>
       <c r="AV5" s="9">
         <f t="shared" si="0"/>
-        <v>45198</v>
+        <v>45261</v>
       </c>
       <c r="AW5" s="9">
         <f t="shared" si="0"/>
-        <v>45199</v>
+        <v>45262</v>
       </c>
       <c r="AX5" s="11">
         <f t="shared" si="0"/>
-        <v>45200</v>
+        <v>45263</v>
       </c>
       <c r="AY5" s="10">
         <f>AX5+1</f>
-        <v>45201</v>
+        <v>45264</v>
       </c>
       <c r="AZ5" s="9">
         <f>AY5+1</f>
-        <v>45202</v>
+        <v>45265</v>
       </c>
       <c r="BA5" s="9">
         <f t="shared" ref="BA5:BE5" si="1">AZ5+1</f>
-        <v>45203</v>
+        <v>45266</v>
       </c>
       <c r="BB5" s="9">
         <f t="shared" si="1"/>
-        <v>45204</v>
+        <v>45267</v>
       </c>
       <c r="BC5" s="9">
         <f t="shared" si="1"/>
-        <v>45205</v>
+        <v>45268</v>
       </c>
       <c r="BD5" s="9">
         <f t="shared" si="1"/>
-        <v>45206</v>
+        <v>45269</v>
       </c>
       <c r="BE5" s="11">
         <f t="shared" si="1"/>
-        <v>45207</v>
+        <v>45270</v>
       </c>
       <c r="BF5" s="10">
         <f>BE5+1</f>
-        <v>45208</v>
+        <v>45271</v>
       </c>
       <c r="BG5" s="9">
         <f>BF5+1</f>
-        <v>45209</v>
+        <v>45272</v>
       </c>
       <c r="BH5" s="9">
         <f t="shared" ref="BH5:BL5" si="2">BG5+1</f>
-        <v>45210</v>
+        <v>45273</v>
       </c>
       <c r="BI5" s="9">
         <f t="shared" si="2"/>
-        <v>45211</v>
+        <v>45274</v>
       </c>
       <c r="BJ5" s="9">
         <f t="shared" si="2"/>
-        <v>45212</v>
+        <v>45275</v>
       </c>
       <c r="BK5" s="9">
         <f t="shared" si="2"/>
-        <v>45213</v>
+        <v>45276</v>
       </c>
       <c r="BL5" s="11">
         <f t="shared" si="2"/>
-        <v>45214</v>
+        <v>45277</v>
       </c>
       <c r="BM5" s="10">
         <f>BL5+1</f>
-        <v>45215</v>
+        <v>45278</v>
       </c>
       <c r="BN5" s="9">
         <f>BM5+1</f>
-        <v>45216</v>
+        <v>45279</v>
       </c>
       <c r="BO5" s="9">
         <f t="shared" ref="BO5" si="3">BN5+1</f>
-        <v>45217</v>
+        <v>45280</v>
       </c>
       <c r="BP5" s="9">
         <f t="shared" ref="BP5" si="4">BO5+1</f>
-        <v>45218</v>
+        <v>45281</v>
       </c>
       <c r="BQ5" s="9">
         <f t="shared" ref="BQ5" si="5">BP5+1</f>
-        <v>45219</v>
+        <v>45282</v>
       </c>
       <c r="BR5" s="9">
         <f t="shared" ref="BR5" si="6">BQ5+1</f>
-        <v>45220</v>
+        <v>45283</v>
       </c>
       <c r="BS5" s="11">
         <f t="shared" ref="BS5" si="7">BR5+1</f>
-        <v>45221</v>
+        <v>45284</v>
       </c>
       <c r="BT5" s="10">
         <f>BS5+1</f>
-        <v>45222</v>
+        <v>45285</v>
       </c>
       <c r="BU5" s="9">
         <f>BT5+1</f>
-        <v>45223</v>
+        <v>45286</v>
       </c>
       <c r="BV5" s="9">
         <f t="shared" ref="BV5" si="8">BU5+1</f>
-        <v>45224</v>
+        <v>45287</v>
       </c>
       <c r="BW5" s="9">
         <f t="shared" ref="BW5" si="9">BV5+1</f>
-        <v>45225</v>
+        <v>45288</v>
       </c>
       <c r="BX5" s="9">
         <f t="shared" ref="BX5" si="10">BW5+1</f>
-        <v>45226</v>
+        <v>45289</v>
       </c>
       <c r="BY5" s="9">
         <f t="shared" ref="BY5" si="11">BX5+1</f>
-        <v>45227</v>
+        <v>45290</v>
       </c>
       <c r="BZ5" s="11">
         <f t="shared" ref="BZ5" si="12">BY5+1</f>
-        <v>45228</v>
+        <v>45291</v>
       </c>
       <c r="CA5" s="10">
         <f>BZ5+1</f>
-        <v>45229</v>
+        <v>45292</v>
       </c>
       <c r="CB5" s="9">
         <f>CA5+1</f>
-        <v>45230</v>
+        <v>45293</v>
       </c>
       <c r="CC5" s="9">
         <f t="shared" ref="CC5" si="13">CB5+1</f>
-        <v>45231</v>
+        <v>45294</v>
       </c>
       <c r="CD5" s="9">
         <f t="shared" ref="CD5" si="14">CC5+1</f>
-        <v>45232</v>
+        <v>45295</v>
       </c>
       <c r="CE5" s="9">
         <f t="shared" ref="CE5" si="15">CD5+1</f>
-        <v>45233</v>
+        <v>45296</v>
       </c>
       <c r="CF5" s="9">
         <f t="shared" ref="CF5" si="16">CE5+1</f>
-        <v>45234</v>
+        <v>45297</v>
       </c>
       <c r="CG5" s="11">
         <f t="shared" ref="CG5" si="17">CF5+1</f>
-        <v>45235</v>
+        <v>45298</v>
       </c>
       <c r="CH5" s="10">
         <f>CG5+1</f>
-        <v>45236</v>
+        <v>45299</v>
       </c>
       <c r="CI5" s="9">
         <f>CH5+1</f>
-        <v>45237</v>
+        <v>45300</v>
       </c>
       <c r="CJ5" s="9">
         <f t="shared" ref="CJ5" si="18">CI5+1</f>
-        <v>45238</v>
+        <v>45301</v>
       </c>
       <c r="CK5" s="9">
         <f t="shared" ref="CK5" si="19">CJ5+1</f>
-        <v>45239</v>
+        <v>45302</v>
       </c>
       <c r="CL5" s="9">
         <f t="shared" ref="CL5" si="20">CK5+1</f>
-        <v>45240</v>
+        <v>45303</v>
       </c>
       <c r="CM5" s="9">
         <f t="shared" ref="CM5" si="21">CL5+1</f>
-        <v>45241</v>
+        <v>45304</v>
       </c>
       <c r="CN5" s="11">
         <f t="shared" ref="CN5" si="22">CM5+1</f>
-        <v>45242</v>
+        <v>45305</v>
       </c>
       <c r="CO5" s="10">
         <f>CN5+1</f>
-        <v>45243</v>
+        <v>45306</v>
       </c>
       <c r="CP5" s="9">
         <f>CO5+1</f>
-        <v>45244</v>
+        <v>45307</v>
       </c>
       <c r="CQ5" s="9">
         <f t="shared" ref="CQ5" si="23">CP5+1</f>
-        <v>45245</v>
+        <v>45308</v>
       </c>
       <c r="CR5" s="9">
         <f t="shared" ref="CR5" si="24">CQ5+1</f>
-        <v>45246</v>
+        <v>45309</v>
       </c>
       <c r="CS5" s="9">
         <f t="shared" ref="CS5" si="25">CR5+1</f>
-        <v>45247</v>
+        <v>45310</v>
       </c>
       <c r="CT5" s="9">
         <f t="shared" ref="CT5" si="26">CS5+1</f>
-        <v>45248</v>
+        <v>45311</v>
       </c>
       <c r="CU5" s="11">
         <f t="shared" ref="CU5" si="27">CT5+1</f>
-        <v>45249</v>
+        <v>45312</v>
       </c>
       <c r="CV5" s="10">
         <f>CU5+1</f>
-        <v>45250</v>
+        <v>45313</v>
       </c>
       <c r="CW5" s="9">
         <f>CV5+1</f>
-        <v>45251</v>
+        <v>45314</v>
       </c>
       <c r="CX5" s="9">
         <f t="shared" ref="CX5" si="28">CW5+1</f>
-        <v>45252</v>
+        <v>45315</v>
       </c>
       <c r="CY5" s="9">
         <f t="shared" ref="CY5" si="29">CX5+1</f>
-        <v>45253</v>
+        <v>45316</v>
       </c>
       <c r="CZ5" s="9">
         <f t="shared" ref="CZ5" si="30">CY5+1</f>
-        <v>45254</v>
+        <v>45317</v>
       </c>
       <c r="DA5" s="9">
         <f t="shared" ref="DA5" si="31">CZ5+1</f>
-        <v>45255</v>
+        <v>45318</v>
       </c>
       <c r="DB5" s="11">
         <f t="shared" ref="DB5" si="32">DA5+1</f>
-        <v>45256</v>
+        <v>45319</v>
       </c>
     </row>
     <row r="6" spans="1:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3167,7 +3159,7 @@
       <c r="F8" s="18"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14" t="str">
-        <f t="shared" ref="H8:H57" si="37">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H59" si="37">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="41"/>
@@ -3274,10 +3266,10 @@
         <v>17</v>
       </c>
       <c r="B9" s="74" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="67" t="s">
         <v>46</v>
-      </c>
-      <c r="C9" s="67" t="s">
-        <v>51</v>
       </c>
       <c r="D9" s="19">
         <v>1</v>
@@ -3399,10 +3391,10 @@
         <v>18</v>
       </c>
       <c r="B10" s="74" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C10" s="67" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D10" s="19">
         <v>1</v>
@@ -3522,10 +3514,10 @@
     <row r="11" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="55"/>
       <c r="B11" s="74" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C11" s="67" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D11" s="19">
         <v>1</v>
@@ -3645,10 +3637,10 @@
     <row r="12" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="55"/>
       <c r="B12" s="74" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C12" s="67" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D12" s="19">
         <v>1</v>
@@ -3986,10 +3978,10 @@
     </row>
     <row r="15" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="56" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C15" s="68"/>
       <c r="D15" s="21"/>
@@ -4102,10 +4094,10 @@
     <row r="16" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="56"/>
       <c r="B16" s="75" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C16" s="83" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D16" s="24">
         <v>1</v>
@@ -4225,10 +4217,10 @@
     <row r="17" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="55"/>
       <c r="B17" s="75" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="83" t="s">
         <v>46</v>
-      </c>
-      <c r="C17" s="83" t="s">
-        <v>51</v>
       </c>
       <c r="D17" s="24">
         <v>1</v>
@@ -4348,10 +4340,10 @@
     <row r="18" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="55"/>
       <c r="B18" s="75" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C18" s="69" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D18" s="24">
         <v>1</v>
@@ -4471,10 +4463,10 @@
     <row r="19" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="55"/>
       <c r="B19" s="75" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C19" s="69" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D19" s="24">
         <v>1</v>
@@ -4594,10 +4586,10 @@
     <row r="20" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="55"/>
       <c r="B20" s="75" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C20" s="69" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D20" s="24">
         <v>1</v>
@@ -4716,13 +4708,13 @@
     </row>
     <row r="21" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="55" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B21" s="75" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C21" s="69" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D21" s="24">
         <v>1</v>
@@ -4842,10 +4834,10 @@
     <row r="22" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="55"/>
       <c r="B22" s="75" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C22" s="69" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D22" s="24">
         <v>1</v>
@@ -4965,10 +4957,10 @@
     <row r="23" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="55"/>
       <c r="B23" s="75" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C23" s="69" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D23" s="24">
         <v>1</v>
@@ -5088,10 +5080,10 @@
     <row r="24" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="55"/>
       <c r="B24" s="75" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C24" s="69" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D24" s="24">
         <v>1</v>
@@ -5211,10 +5203,10 @@
     <row r="25" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="55"/>
       <c r="B25" s="75" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C25" s="69" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D25" s="24">
         <v>1</v>
@@ -5334,10 +5326,10 @@
     <row r="26" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="55"/>
       <c r="B26" s="75" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C26" s="69" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D26" s="24">
         <v>1</v>
@@ -5567,7 +5559,7 @@
     </row>
     <row r="28" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="55" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B28" s="75"/>
       <c r="C28" s="69"/>
@@ -5680,7 +5672,7 @@
     </row>
     <row r="29" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C29" s="70"/>
       <c r="D29" s="26"/>
@@ -5792,21 +5784,21 @@
     </row>
     <row r="30" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="76" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C30" s="84" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D30" s="29">
         <v>1</v>
       </c>
       <c r="E30" s="63">
-        <f>E46</f>
-        <v>45222</v>
+        <f>E48</f>
+        <v>45233</v>
       </c>
       <c r="F30" s="63">
         <f>E30+11</f>
-        <v>45233</v>
+        <v>45244</v>
       </c>
       <c r="G30" s="14"/>
       <c r="H30" s="14">
@@ -5914,10 +5906,10 @@
     </row>
     <row r="31" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="76" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="84" t="s">
         <v>46</v>
-      </c>
-      <c r="C31" s="84" t="s">
-        <v>51</v>
       </c>
       <c r="D31" s="29">
         <v>1</v>
@@ -6036,10 +6028,10 @@
     </row>
     <row r="32" spans="1:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="76" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C32" s="84" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D32" s="29">
         <v>1</v>
@@ -6158,10 +6150,10 @@
     </row>
     <row r="33" spans="2:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="85" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C33" s="84" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D33" s="29">
         <v>1</v>
@@ -6277,10 +6269,10 @@
     </row>
     <row r="34" spans="2:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="85" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C34" s="84" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D34" s="29">
         <v>1</v>
@@ -6399,10 +6391,10 @@
     </row>
     <row r="35" spans="2:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="85" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C35" s="84" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D35" s="29">
         <v>1</v>
@@ -6518,10 +6510,10 @@
     </row>
     <row r="36" spans="2:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="85" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C36" s="84" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D36" s="29">
         <v>1</v>
@@ -6637,10 +6629,10 @@
     </row>
     <row r="37" spans="2:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B37" s="85" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C37" s="84" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D37" s="29">
         <v>1</v>
@@ -6756,10 +6748,10 @@
     </row>
     <row r="38" spans="2:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="85" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C38" s="84" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D38" s="29">
         <v>1</v>
@@ -6875,10 +6867,10 @@
     </row>
     <row r="39" spans="2:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" s="85" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C39" s="84" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D39" s="29">
         <v>0.4</v>
@@ -6994,10 +6986,10 @@
     </row>
     <row r="40" spans="2:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B40" s="85" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C40" s="84" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D40" s="29">
         <v>1</v>
@@ -7113,10 +7105,10 @@
     </row>
     <row r="41" spans="2:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B41" s="85" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C41" s="84" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D41" s="29">
         <v>0.5</v>
@@ -7232,10 +7224,10 @@
     </row>
     <row r="42" spans="2:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B42" s="85" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C42" s="84" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D42" s="29">
         <v>0.4</v>
@@ -7563,19 +7555,14 @@
       <c r="DA44" s="41"/>
       <c r="DB44" s="41"/>
     </row>
-    <row r="45" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="C45" s="71"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="33"/>
+    <row r="45" spans="2:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B45" s="85"/>
+      <c r="C45" s="84"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="63"/>
+      <c r="F45" s="63"/>
       <c r="G45" s="14"/>
-      <c r="H45" s="14" t="str">
-        <f t="shared" si="37"/>
-        <v/>
-      </c>
+      <c r="H45" s="14"/>
       <c r="I45" s="41"/>
       <c r="J45" s="41"/>
       <c r="K45" s="41"/>
@@ -7675,29 +7662,14 @@
       <c r="DA45" s="41"/>
       <c r="DB45" s="41"/>
     </row>
-    <row r="46" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="86" t="s">
-        <v>78</v>
-      </c>
-      <c r="C46" s="87" t="s">
-        <v>51</v>
-      </c>
-      <c r="D46" s="34">
-        <v>1</v>
-      </c>
-      <c r="E46" s="88">
-        <f>Project_Start+ 63</f>
-        <v>45222</v>
-      </c>
-      <c r="F46" s="88">
-        <f>E46+35</f>
-        <v>45257</v>
-      </c>
+    <row r="46" spans="2:106" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="85"/>
+      <c r="C46" s="84"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="63"/>
+      <c r="F46" s="63"/>
       <c r="G46" s="14"/>
-      <c r="H46" s="14">
-        <f t="shared" si="37"/>
-        <v>36</v>
-      </c>
+      <c r="H46" s="14"/>
       <c r="I46" s="41"/>
       <c r="J46" s="41"/>
       <c r="K46" s="41"/>
@@ -7798,19 +7770,18 @@
       <c r="DB46" s="41"/>
     </row>
     <row r="47" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="86" t="s">
-        <v>79</v>
-      </c>
-      <c r="C47" s="87" t="s">
-        <v>64</v>
-      </c>
-      <c r="D47" s="34">
-        <v>1</v>
-      </c>
-      <c r="E47" s="64"/>
-      <c r="F47" s="64"/>
+      <c r="B47" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C47" s="71"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="33"/>
       <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
+      <c r="H47" s="14" t="str">
+        <f t="shared" si="37"/>
+        <v/>
+      </c>
       <c r="I47" s="41"/>
       <c r="J47" s="41"/>
       <c r="K47" s="41"/>
@@ -7912,18 +7883,27 @@
     </row>
     <row r="48" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B48" s="86" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C48" s="87" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="D48" s="34">
-        <v>0.2</v>
-      </c>
-      <c r="E48" s="64"/>
-      <c r="F48" s="64"/>
+        <v>0.5</v>
+      </c>
+      <c r="E48" s="88">
+        <f>Project_Start+ 74</f>
+        <v>45233</v>
+      </c>
+      <c r="F48" s="88">
+        <f>E48+24</f>
+        <v>45257</v>
+      </c>
       <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
+      <c r="H48" s="14">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
       <c r="I48" s="41"/>
       <c r="J48" s="41"/>
       <c r="K48" s="41"/>
@@ -8025,16 +8005,22 @@
     </row>
     <row r="49" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B49" s="86" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C49" s="87" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D49" s="34">
-        <v>0.5</v>
-      </c>
-      <c r="E49" s="64"/>
-      <c r="F49" s="64"/>
+        <v>1</v>
+      </c>
+      <c r="E49" s="64">
+        <f>Project_Start+ 63</f>
+        <v>45222</v>
+      </c>
+      <c r="F49" s="64">
+        <f>E49+20</f>
+        <v>45242</v>
+      </c>
       <c r="G49" s="14"/>
       <c r="H49" s="14"/>
       <c r="I49" s="41"/>
@@ -8138,16 +8124,22 @@
     </row>
     <row r="50" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B50" s="86" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C50" s="87" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D50" s="34">
-        <v>0.6</v>
-      </c>
-      <c r="E50" s="64"/>
-      <c r="F50" s="64"/>
+        <v>0.2</v>
+      </c>
+      <c r="E50" s="64">
+        <f>Project_Start+87</f>
+        <v>45246</v>
+      </c>
+      <c r="F50" s="64">
+        <f>E50+11</f>
+        <v>45257</v>
+      </c>
       <c r="G50" s="14"/>
       <c r="H50" s="14"/>
       <c r="I50" s="41"/>
@@ -8251,16 +8243,22 @@
     </row>
     <row r="51" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B51" s="86" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C51" s="87" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D51" s="34">
-        <v>0.9</v>
-      </c>
-      <c r="E51" s="64"/>
-      <c r="F51" s="64"/>
+        <v>0.5</v>
+      </c>
+      <c r="E51" s="64">
+        <f>Project_Start+87</f>
+        <v>45246</v>
+      </c>
+      <c r="F51" s="64">
+        <f>E51+11</f>
+        <v>45257</v>
+      </c>
       <c r="G51" s="14"/>
       <c r="H51" s="14"/>
       <c r="I51" s="41"/>
@@ -8364,16 +8362,22 @@
     </row>
     <row r="52" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B52" s="86" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C52" s="87" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="D52" s="34">
         <v>0.6</v>
       </c>
-      <c r="E52" s="64"/>
-      <c r="F52" s="64"/>
+      <c r="E52" s="64">
+        <f>Project_Start+ 63</f>
+        <v>45222</v>
+      </c>
+      <c r="F52" s="64">
+        <f>E52+35</f>
+        <v>45257</v>
+      </c>
       <c r="G52" s="14"/>
       <c r="H52" s="14"/>
       <c r="I52" s="41"/>
@@ -8476,11 +8480,23 @@
       <c r="DB52" s="41"/>
     </row>
     <row r="53" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="77"/>
-      <c r="C53" s="72"/>
-      <c r="D53" s="34"/>
-      <c r="E53" s="64"/>
-      <c r="F53" s="64"/>
+      <c r="B53" s="86" t="s">
+        <v>77</v>
+      </c>
+      <c r="C53" s="87" t="s">
+        <v>59</v>
+      </c>
+      <c r="D53" s="34">
+        <v>0.9</v>
+      </c>
+      <c r="E53" s="64">
+        <f>Project_Start+64</f>
+        <v>45223</v>
+      </c>
+      <c r="F53" s="64">
+        <f>E53+34</f>
+        <v>45257</v>
+      </c>
       <c r="G53" s="14"/>
       <c r="H53" s="14"/>
       <c r="I53" s="41"/>
@@ -8583,22 +8599,25 @@
       <c r="DB53" s="41"/>
     </row>
     <row r="54" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="77" t="s">
-        <v>25</v>
-      </c>
-      <c r="C54" s="72"/>
-      <c r="D54" s="34"/>
-      <c r="E54" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="F54" s="64" t="s">
-        <v>28</v>
+      <c r="B54" s="86" t="s">
+        <v>78</v>
+      </c>
+      <c r="C54" s="87" t="s">
+        <v>65</v>
+      </c>
+      <c r="D54" s="34">
+        <v>0.6</v>
+      </c>
+      <c r="E54" s="64">
+        <f>Project_Start+ 63</f>
+        <v>45222</v>
+      </c>
+      <c r="F54" s="64">
+        <f>E54+35</f>
+        <v>45257</v>
       </c>
       <c r="G54" s="14"/>
-      <c r="H54" s="14" t="e">
-        <f t="shared" si="37"/>
-        <v>#VALUE!</v>
-      </c>
+      <c r="H54" s="14"/>
       <c r="I54" s="41"/>
       <c r="J54" s="41"/>
       <c r="K54" s="41"/>
@@ -8699,22 +8718,25 @@
       <c r="DB54" s="41"/>
     </row>
     <row r="55" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="77" t="s">
-        <v>26</v>
-      </c>
-      <c r="C55" s="72"/>
-      <c r="D55" s="34"/>
-      <c r="E55" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="F55" s="64" t="s">
-        <v>28</v>
+      <c r="B55" s="86" t="s">
+        <v>79</v>
+      </c>
+      <c r="C55" s="87" t="s">
+        <v>46</v>
+      </c>
+      <c r="D55" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="E55" s="64">
+        <f>Project_Start+92</f>
+        <v>45251</v>
+      </c>
+      <c r="F55" s="64">
+        <f>E55+10</f>
+        <v>45261</v>
       </c>
       <c r="G55" s="14"/>
-      <c r="H55" s="14" t="e">
-        <f t="shared" si="37"/>
-        <v>#VALUE!</v>
-      </c>
+      <c r="H55" s="14"/>
       <c r="I55" s="41"/>
       <c r="J55" s="41"/>
       <c r="K55" s="41"/>
@@ -8815,21 +8837,27 @@
       <c r="DB55" s="41"/>
     </row>
     <row r="56" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="77" t="s">
-        <v>19</v>
-      </c>
-      <c r="C56" s="72"/>
-      <c r="D56" s="34"/>
-      <c r="E56" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="F56" s="64" t="s">
-        <v>28</v>
+      <c r="B56" s="86" t="s">
+        <v>80</v>
+      </c>
+      <c r="C56" s="87" t="s">
+        <v>46</v>
+      </c>
+      <c r="D56" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="E56" s="64">
+        <f>Project_Start+92</f>
+        <v>45251</v>
+      </c>
+      <c r="F56" s="88">
+        <f>E56+10</f>
+        <v>45261</v>
       </c>
       <c r="G56" s="14"/>
-      <c r="H56" s="14" t="e">
+      <c r="H56" s="14">
         <f t="shared" si="37"/>
-        <v>#VALUE!</v>
+        <v>11</v>
       </c>
       <c r="I56" s="41"/>
       <c r="J56" s="41"/>
@@ -8931,21 +8959,27 @@
       <c r="DB56" s="41"/>
     </row>
     <row r="57" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="77" t="s">
-        <v>20</v>
-      </c>
-      <c r="C57" s="72"/>
-      <c r="D57" s="34"/>
-      <c r="E57" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="F57" s="64" t="s">
-        <v>28</v>
+      <c r="B57" s="86" t="s">
+        <v>42</v>
+      </c>
+      <c r="C57" s="87" t="s">
+        <v>81</v>
+      </c>
+      <c r="D57" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="E57" s="64">
+        <f>Project_Start+92</f>
+        <v>45251</v>
+      </c>
+      <c r="F57" s="64">
+        <f>E57+10</f>
+        <v>45261</v>
       </c>
       <c r="G57" s="14"/>
-      <c r="H57" s="14" t="e">
+      <c r="H57" s="14">
         <f t="shared" si="37"/>
-        <v>#VALUE!</v>
+        <v>11</v>
       </c>
       <c r="I57" s="41"/>
       <c r="J57" s="41"/>
@@ -9046,463 +9080,695 @@
       <c r="DA57" s="41"/>
       <c r="DB57" s="41"/>
     </row>
-    <row r="58" spans="2:106" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
-      <c r="H58" s="3"/>
-      <c r="I58" s="3"/>
-      <c r="J58" s="3"/>
-      <c r="K58" s="3"/>
-      <c r="L58" s="3"/>
-      <c r="M58" s="3"/>
-      <c r="N58" s="3"/>
-      <c r="O58" s="3"/>
-      <c r="P58" s="3"/>
-      <c r="Q58" s="3"/>
-      <c r="R58" s="3"/>
-      <c r="S58" s="3"/>
-      <c r="T58" s="3"/>
-      <c r="U58" s="3"/>
-      <c r="V58" s="3"/>
-      <c r="W58" s="3"/>
-      <c r="X58" s="3"/>
-      <c r="Y58" s="3"/>
-      <c r="Z58" s="3"/>
-      <c r="AA58" s="3"/>
-      <c r="AB58" s="3"/>
-      <c r="AC58" s="3"/>
-      <c r="AD58" s="3"/>
-      <c r="AE58" s="3"/>
-      <c r="AF58" s="3"/>
-      <c r="AG58" s="3"/>
-      <c r="AH58" s="3"/>
-      <c r="AI58" s="3"/>
-      <c r="AJ58" s="3"/>
-      <c r="AK58" s="3"/>
-      <c r="AL58" s="3"/>
-      <c r="AM58" s="3"/>
-      <c r="AN58" s="3"/>
-      <c r="AO58" s="3"/>
-      <c r="AP58" s="3"/>
-      <c r="AQ58" s="3"/>
-      <c r="AR58" s="3"/>
-      <c r="AS58" s="3"/>
-      <c r="AT58" s="3"/>
-      <c r="AU58" s="3"/>
-      <c r="AV58" s="3"/>
-      <c r="AW58" s="3"/>
-      <c r="AX58" s="3"/>
-      <c r="AY58" s="3"/>
-      <c r="AZ58" s="3"/>
-      <c r="BA58" s="3"/>
-      <c r="BB58" s="3"/>
-      <c r="BC58" s="3"/>
-      <c r="BD58" s="3"/>
-      <c r="BE58" s="3"/>
-      <c r="BF58" s="3"/>
-      <c r="BG58" s="3"/>
-      <c r="BH58" s="3"/>
-      <c r="BI58" s="3"/>
-      <c r="BJ58" s="3"/>
-      <c r="BK58" s="3"/>
-      <c r="BL58" s="3"/>
-      <c r="BM58" s="3"/>
-      <c r="BN58" s="3"/>
-      <c r="BO58" s="3"/>
-      <c r="BP58" s="3"/>
-      <c r="BQ58" s="3"/>
-      <c r="BR58" s="3"/>
-      <c r="BS58" s="3"/>
-      <c r="BT58" s="3"/>
-      <c r="BU58" s="3"/>
-      <c r="BV58" s="3"/>
-      <c r="BW58" s="3"/>
-      <c r="BX58" s="3"/>
-      <c r="BY58" s="3"/>
-      <c r="BZ58" s="3"/>
-      <c r="CA58" s="3"/>
-      <c r="CB58" s="3"/>
-      <c r="CC58" s="3"/>
-      <c r="CD58" s="3"/>
-      <c r="CE58" s="3"/>
-      <c r="CF58" s="3"/>
-      <c r="CG58" s="3"/>
-      <c r="CH58" s="3"/>
-      <c r="CI58" s="3"/>
-      <c r="CJ58" s="3"/>
-      <c r="CK58" s="3"/>
-      <c r="CL58" s="3"/>
-      <c r="CM58" s="3"/>
-      <c r="CN58" s="3"/>
-      <c r="CO58" s="3"/>
-      <c r="CP58" s="3"/>
-      <c r="CQ58" s="3"/>
-      <c r="CR58" s="3"/>
-      <c r="CS58" s="3"/>
-      <c r="CT58" s="3"/>
-      <c r="CU58" s="3"/>
-      <c r="CV58" s="3"/>
-      <c r="CW58" s="3"/>
-      <c r="CX58" s="3"/>
-      <c r="CY58" s="3"/>
-      <c r="CZ58" s="3"/>
-      <c r="DA58" s="3"/>
-      <c r="DB58" s="3"/>
+    <row r="58" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="86" t="s">
+        <v>48</v>
+      </c>
+      <c r="C58" s="87" t="s">
+        <v>46</v>
+      </c>
+      <c r="D58" s="34">
+        <v>0</v>
+      </c>
+      <c r="E58" s="64">
+        <f>Project_Start+92</f>
+        <v>45251</v>
+      </c>
+      <c r="F58" s="64">
+        <f>E58+10</f>
+        <v>45261</v>
+      </c>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14">
+        <f t="shared" si="37"/>
+        <v>11</v>
+      </c>
+      <c r="I58" s="41"/>
+      <c r="J58" s="41"/>
+      <c r="K58" s="41"/>
+      <c r="L58" s="41"/>
+      <c r="M58" s="41"/>
+      <c r="N58" s="41"/>
+      <c r="O58" s="41"/>
+      <c r="P58" s="41"/>
+      <c r="Q58" s="41"/>
+      <c r="R58" s="41"/>
+      <c r="S58" s="41"/>
+      <c r="T58" s="41"/>
+      <c r="U58" s="41"/>
+      <c r="V58" s="41"/>
+      <c r="W58" s="41"/>
+      <c r="X58" s="41"/>
+      <c r="Y58" s="41"/>
+      <c r="Z58" s="41"/>
+      <c r="AA58" s="41"/>
+      <c r="AB58" s="41"/>
+      <c r="AC58" s="41"/>
+      <c r="AD58" s="41"/>
+      <c r="AE58" s="41"/>
+      <c r="AF58" s="41"/>
+      <c r="AG58" s="41"/>
+      <c r="AH58" s="41"/>
+      <c r="AI58" s="41"/>
+      <c r="AJ58" s="41"/>
+      <c r="AK58" s="41"/>
+      <c r="AL58" s="41"/>
+      <c r="AM58" s="41"/>
+      <c r="AN58" s="41"/>
+      <c r="AO58" s="41"/>
+      <c r="AP58" s="41"/>
+      <c r="AQ58" s="41"/>
+      <c r="AR58" s="41"/>
+      <c r="AS58" s="41"/>
+      <c r="AT58" s="41"/>
+      <c r="AU58" s="41"/>
+      <c r="AV58" s="41"/>
+      <c r="AW58" s="41"/>
+      <c r="AX58" s="41"/>
+      <c r="AY58" s="41"/>
+      <c r="AZ58" s="41"/>
+      <c r="BA58" s="41"/>
+      <c r="BB58" s="41"/>
+      <c r="BC58" s="41"/>
+      <c r="BD58" s="41"/>
+      <c r="BE58" s="41"/>
+      <c r="BF58" s="41"/>
+      <c r="BG58" s="41"/>
+      <c r="BH58" s="41"/>
+      <c r="BI58" s="41"/>
+      <c r="BJ58" s="41"/>
+      <c r="BK58" s="41"/>
+      <c r="BL58" s="41"/>
+      <c r="BM58" s="41"/>
+      <c r="BN58" s="41"/>
+      <c r="BO58" s="41"/>
+      <c r="BP58" s="41"/>
+      <c r="BQ58" s="41"/>
+      <c r="BR58" s="41"/>
+      <c r="BS58" s="41"/>
+      <c r="BT58" s="41"/>
+      <c r="BU58" s="41"/>
+      <c r="BV58" s="41"/>
+      <c r="BW58" s="41"/>
+      <c r="BX58" s="41"/>
+      <c r="BY58" s="41"/>
+      <c r="BZ58" s="41"/>
+      <c r="CA58" s="41"/>
+      <c r="CB58" s="41"/>
+      <c r="CC58" s="41"/>
+      <c r="CD58" s="41"/>
+      <c r="CE58" s="41"/>
+      <c r="CF58" s="41"/>
+      <c r="CG58" s="41"/>
+      <c r="CH58" s="41"/>
+      <c r="CI58" s="41"/>
+      <c r="CJ58" s="41"/>
+      <c r="CK58" s="41"/>
+      <c r="CL58" s="41"/>
+      <c r="CM58" s="41"/>
+      <c r="CN58" s="41"/>
+      <c r="CO58" s="41"/>
+      <c r="CP58" s="41"/>
+      <c r="CQ58" s="41"/>
+      <c r="CR58" s="41"/>
+      <c r="CS58" s="41"/>
+      <c r="CT58" s="41"/>
+      <c r="CU58" s="41"/>
+      <c r="CV58" s="41"/>
+      <c r="CW58" s="41"/>
+      <c r="CX58" s="41"/>
+      <c r="CY58" s="41"/>
+      <c r="CZ58" s="41"/>
+      <c r="DA58" s="41"/>
+      <c r="DB58" s="41"/>
     </row>
     <row r="59" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-      <c r="H59" s="3"/>
-      <c r="I59" s="3"/>
-      <c r="J59" s="3"/>
-      <c r="K59" s="3"/>
-      <c r="L59" s="3"/>
-      <c r="M59" s="3"/>
-      <c r="N59" s="3"/>
-      <c r="O59" s="3"/>
-      <c r="P59" s="3"/>
-      <c r="Q59" s="3"/>
-      <c r="R59" s="3"/>
-      <c r="S59" s="3"/>
-      <c r="T59" s="3"/>
-      <c r="U59" s="3"/>
-      <c r="V59" s="3"/>
-      <c r="W59" s="3"/>
-      <c r="X59" s="3"/>
-      <c r="Y59" s="3"/>
-      <c r="Z59" s="3"/>
-      <c r="AA59" s="3"/>
-      <c r="AB59" s="3"/>
-      <c r="AC59" s="3"/>
-      <c r="AD59" s="3"/>
-      <c r="AE59" s="3"/>
-      <c r="AF59" s="3"/>
-      <c r="AG59" s="3"/>
-      <c r="AH59" s="3"/>
-      <c r="AI59" s="3"/>
-      <c r="AJ59" s="3"/>
-      <c r="AK59" s="3"/>
-      <c r="AL59" s="3"/>
-      <c r="AM59" s="3"/>
-      <c r="AN59" s="3"/>
-      <c r="AO59" s="3"/>
-      <c r="AP59" s="3"/>
-      <c r="AQ59" s="3"/>
-      <c r="AR59" s="3"/>
-      <c r="AS59" s="3"/>
-      <c r="AT59" s="3"/>
-      <c r="AU59" s="3"/>
-      <c r="AV59" s="3"/>
-      <c r="AW59" s="3"/>
-      <c r="AX59" s="3"/>
-      <c r="AY59" s="3"/>
-      <c r="AZ59" s="3"/>
-      <c r="BA59" s="3"/>
-      <c r="BB59" s="3"/>
-      <c r="BC59" s="3"/>
-      <c r="BD59" s="3"/>
-      <c r="BE59" s="3"/>
-      <c r="BF59" s="3"/>
-      <c r="BG59" s="3"/>
-      <c r="BH59" s="3"/>
-      <c r="BI59" s="3"/>
-      <c r="BJ59" s="3"/>
-      <c r="BK59" s="3"/>
-      <c r="BL59" s="3"/>
-      <c r="BM59" s="3"/>
-      <c r="BN59" s="3"/>
-      <c r="BO59" s="3"/>
-      <c r="BP59" s="3"/>
-      <c r="BQ59" s="3"/>
-      <c r="BR59" s="3"/>
-      <c r="BS59" s="3"/>
-      <c r="BT59" s="3"/>
-      <c r="BU59" s="3"/>
-      <c r="BV59" s="3"/>
-      <c r="BW59" s="3"/>
-      <c r="BX59" s="3"/>
-      <c r="BY59" s="3"/>
-      <c r="BZ59" s="3"/>
-      <c r="CA59" s="3"/>
-      <c r="CB59" s="3"/>
-      <c r="CC59" s="3"/>
-      <c r="CD59" s="3"/>
-      <c r="CE59" s="3"/>
-      <c r="CF59" s="3"/>
-      <c r="CG59" s="3"/>
-      <c r="CH59" s="3"/>
-      <c r="CI59" s="3"/>
-      <c r="CJ59" s="3"/>
-      <c r="CK59" s="3"/>
-      <c r="CL59" s="3"/>
-      <c r="CM59" s="3"/>
-      <c r="CN59" s="3"/>
-      <c r="CO59" s="3"/>
-      <c r="CP59" s="3"/>
-      <c r="CQ59" s="3"/>
-      <c r="CR59" s="3"/>
-      <c r="CS59" s="3"/>
-      <c r="CT59" s="3"/>
-      <c r="CU59" s="3"/>
-      <c r="CV59" s="3"/>
-      <c r="CW59" s="3"/>
-      <c r="CX59" s="3"/>
-      <c r="CY59" s="3"/>
-      <c r="CZ59" s="3"/>
-      <c r="DA59" s="3"/>
-      <c r="DB59" s="3"/>
+      <c r="B59" s="77"/>
+      <c r="C59" s="72"/>
+      <c r="D59" s="34"/>
+      <c r="E59" s="64"/>
+      <c r="F59" s="64"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="14" t="str">
+        <f t="shared" si="37"/>
+        <v/>
+      </c>
+      <c r="I59" s="41"/>
+      <c r="J59" s="41"/>
+      <c r="K59" s="41"/>
+      <c r="L59" s="41"/>
+      <c r="M59" s="41"/>
+      <c r="N59" s="41"/>
+      <c r="O59" s="41"/>
+      <c r="P59" s="41"/>
+      <c r="Q59" s="41"/>
+      <c r="R59" s="41"/>
+      <c r="S59" s="41"/>
+      <c r="T59" s="41"/>
+      <c r="U59" s="41"/>
+      <c r="V59" s="41"/>
+      <c r="W59" s="41"/>
+      <c r="X59" s="41"/>
+      <c r="Y59" s="41"/>
+      <c r="Z59" s="41"/>
+      <c r="AA59" s="41"/>
+      <c r="AB59" s="41"/>
+      <c r="AC59" s="41"/>
+      <c r="AD59" s="41"/>
+      <c r="AE59" s="41"/>
+      <c r="AF59" s="41"/>
+      <c r="AG59" s="41"/>
+      <c r="AH59" s="41"/>
+      <c r="AI59" s="41"/>
+      <c r="AJ59" s="41"/>
+      <c r="AK59" s="41"/>
+      <c r="AL59" s="41"/>
+      <c r="AM59" s="41"/>
+      <c r="AN59" s="41"/>
+      <c r="AO59" s="41"/>
+      <c r="AP59" s="41"/>
+      <c r="AQ59" s="41"/>
+      <c r="AR59" s="41"/>
+      <c r="AS59" s="41"/>
+      <c r="AT59" s="41"/>
+      <c r="AU59" s="41"/>
+      <c r="AV59" s="41"/>
+      <c r="AW59" s="41"/>
+      <c r="AX59" s="41"/>
+      <c r="AY59" s="41"/>
+      <c r="AZ59" s="41"/>
+      <c r="BA59" s="41"/>
+      <c r="BB59" s="41"/>
+      <c r="BC59" s="41"/>
+      <c r="BD59" s="41"/>
+      <c r="BE59" s="41"/>
+      <c r="BF59" s="41"/>
+      <c r="BG59" s="41"/>
+      <c r="BH59" s="41"/>
+      <c r="BI59" s="41"/>
+      <c r="BJ59" s="41"/>
+      <c r="BK59" s="41"/>
+      <c r="BL59" s="41"/>
+      <c r="BM59" s="41"/>
+      <c r="BN59" s="41"/>
+      <c r="BO59" s="41"/>
+      <c r="BP59" s="41"/>
+      <c r="BQ59" s="41"/>
+      <c r="BR59" s="41"/>
+      <c r="BS59" s="41"/>
+      <c r="BT59" s="41"/>
+      <c r="BU59" s="41"/>
+      <c r="BV59" s="41"/>
+      <c r="BW59" s="41"/>
+      <c r="BX59" s="41"/>
+      <c r="BY59" s="41"/>
+      <c r="BZ59" s="41"/>
+      <c r="CA59" s="41"/>
+      <c r="CB59" s="41"/>
+      <c r="CC59" s="41"/>
+      <c r="CD59" s="41"/>
+      <c r="CE59" s="41"/>
+      <c r="CF59" s="41"/>
+      <c r="CG59" s="41"/>
+      <c r="CH59" s="41"/>
+      <c r="CI59" s="41"/>
+      <c r="CJ59" s="41"/>
+      <c r="CK59" s="41"/>
+      <c r="CL59" s="41"/>
+      <c r="CM59" s="41"/>
+      <c r="CN59" s="41"/>
+      <c r="CO59" s="41"/>
+      <c r="CP59" s="41"/>
+      <c r="CQ59" s="41"/>
+      <c r="CR59" s="41"/>
+      <c r="CS59" s="41"/>
+      <c r="CT59" s="41"/>
+      <c r="CU59" s="41"/>
+      <c r="CV59" s="41"/>
+      <c r="CW59" s="41"/>
+      <c r="CX59" s="41"/>
+      <c r="CY59" s="41"/>
+      <c r="CZ59" s="41"/>
+      <c r="DA59" s="41"/>
+      <c r="DB59" s="41"/>
     </row>
-    <row r="60" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="78"/>
-      <c r="C60" s="73"/>
-      <c r="D60" s="13"/>
-      <c r="E60" s="65"/>
-      <c r="F60" s="65"/>
-      <c r="G60" s="14"/>
-      <c r="H60" s="14" t="str">
+    <row r="60" spans="2:106" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="3"/>
+      <c r="L60" s="3"/>
+      <c r="M60" s="3"/>
+      <c r="N60" s="3"/>
+      <c r="O60" s="3"/>
+      <c r="P60" s="3"/>
+      <c r="Q60" s="3"/>
+      <c r="R60" s="3"/>
+      <c r="S60" s="3"/>
+      <c r="T60" s="3"/>
+      <c r="U60" s="3"/>
+      <c r="V60" s="3"/>
+      <c r="W60" s="3"/>
+      <c r="X60" s="3"/>
+      <c r="Y60" s="3"/>
+      <c r="Z60" s="3"/>
+      <c r="AA60" s="3"/>
+      <c r="AB60" s="3"/>
+      <c r="AC60" s="3"/>
+      <c r="AD60" s="3"/>
+      <c r="AE60" s="3"/>
+      <c r="AF60" s="3"/>
+      <c r="AG60" s="3"/>
+      <c r="AH60" s="3"/>
+      <c r="AI60" s="3"/>
+      <c r="AJ60" s="3"/>
+      <c r="AK60" s="3"/>
+      <c r="AL60" s="3"/>
+      <c r="AM60" s="3"/>
+      <c r="AN60" s="3"/>
+      <c r="AO60" s="3"/>
+      <c r="AP60" s="3"/>
+      <c r="AQ60" s="3"/>
+      <c r="AR60" s="3"/>
+      <c r="AS60" s="3"/>
+      <c r="AT60" s="3"/>
+      <c r="AU60" s="3"/>
+      <c r="AV60" s="3"/>
+      <c r="AW60" s="3"/>
+      <c r="AX60" s="3"/>
+      <c r="AY60" s="3"/>
+      <c r="AZ60" s="3"/>
+      <c r="BA60" s="3"/>
+      <c r="BB60" s="3"/>
+      <c r="BC60" s="3"/>
+      <c r="BD60" s="3"/>
+      <c r="BE60" s="3"/>
+      <c r="BF60" s="3"/>
+      <c r="BG60" s="3"/>
+      <c r="BH60" s="3"/>
+      <c r="BI60" s="3"/>
+      <c r="BJ60" s="3"/>
+      <c r="BK60" s="3"/>
+      <c r="BL60" s="3"/>
+      <c r="BM60" s="3"/>
+      <c r="BN60" s="3"/>
+      <c r="BO60" s="3"/>
+      <c r="BP60" s="3"/>
+      <c r="BQ60" s="3"/>
+      <c r="BR60" s="3"/>
+      <c r="BS60" s="3"/>
+      <c r="BT60" s="3"/>
+      <c r="BU60" s="3"/>
+      <c r="BV60" s="3"/>
+      <c r="BW60" s="3"/>
+      <c r="BX60" s="3"/>
+      <c r="BY60" s="3"/>
+      <c r="BZ60" s="3"/>
+      <c r="CA60" s="3"/>
+      <c r="CB60" s="3"/>
+      <c r="CC60" s="3"/>
+      <c r="CD60" s="3"/>
+      <c r="CE60" s="3"/>
+      <c r="CF60" s="3"/>
+      <c r="CG60" s="3"/>
+      <c r="CH60" s="3"/>
+      <c r="CI60" s="3"/>
+      <c r="CJ60" s="3"/>
+      <c r="CK60" s="3"/>
+      <c r="CL60" s="3"/>
+      <c r="CM60" s="3"/>
+      <c r="CN60" s="3"/>
+      <c r="CO60" s="3"/>
+      <c r="CP60" s="3"/>
+      <c r="CQ60" s="3"/>
+      <c r="CR60" s="3"/>
+      <c r="CS60" s="3"/>
+      <c r="CT60" s="3"/>
+      <c r="CU60" s="3"/>
+      <c r="CV60" s="3"/>
+      <c r="CW60" s="3"/>
+      <c r="CX60" s="3"/>
+      <c r="CY60" s="3"/>
+      <c r="CZ60" s="3"/>
+      <c r="DA60" s="3"/>
+      <c r="DB60" s="3"/>
+    </row>
+    <row r="61" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
+      <c r="K61" s="3"/>
+      <c r="L61" s="3"/>
+      <c r="M61" s="3"/>
+      <c r="N61" s="3"/>
+      <c r="O61" s="3"/>
+      <c r="P61" s="3"/>
+      <c r="Q61" s="3"/>
+      <c r="R61" s="3"/>
+      <c r="S61" s="3"/>
+      <c r="T61" s="3"/>
+      <c r="U61" s="3"/>
+      <c r="V61" s="3"/>
+      <c r="W61" s="3"/>
+      <c r="X61" s="3"/>
+      <c r="Y61" s="3"/>
+      <c r="Z61" s="3"/>
+      <c r="AA61" s="3"/>
+      <c r="AB61" s="3"/>
+      <c r="AC61" s="3"/>
+      <c r="AD61" s="3"/>
+      <c r="AE61" s="3"/>
+      <c r="AF61" s="3"/>
+      <c r="AG61" s="3"/>
+      <c r="AH61" s="3"/>
+      <c r="AI61" s="3"/>
+      <c r="AJ61" s="3"/>
+      <c r="AK61" s="3"/>
+      <c r="AL61" s="3"/>
+      <c r="AM61" s="3"/>
+      <c r="AN61" s="3"/>
+      <c r="AO61" s="3"/>
+      <c r="AP61" s="3"/>
+      <c r="AQ61" s="3"/>
+      <c r="AR61" s="3"/>
+      <c r="AS61" s="3"/>
+      <c r="AT61" s="3"/>
+      <c r="AU61" s="3"/>
+      <c r="AV61" s="3"/>
+      <c r="AW61" s="3"/>
+      <c r="AX61" s="3"/>
+      <c r="AY61" s="3"/>
+      <c r="AZ61" s="3"/>
+      <c r="BA61" s="3"/>
+      <c r="BB61" s="3"/>
+      <c r="BC61" s="3"/>
+      <c r="BD61" s="3"/>
+      <c r="BE61" s="3"/>
+      <c r="BF61" s="3"/>
+      <c r="BG61" s="3"/>
+      <c r="BH61" s="3"/>
+      <c r="BI61" s="3"/>
+      <c r="BJ61" s="3"/>
+      <c r="BK61" s="3"/>
+      <c r="BL61" s="3"/>
+      <c r="BM61" s="3"/>
+      <c r="BN61" s="3"/>
+      <c r="BO61" s="3"/>
+      <c r="BP61" s="3"/>
+      <c r="BQ61" s="3"/>
+      <c r="BR61" s="3"/>
+      <c r="BS61" s="3"/>
+      <c r="BT61" s="3"/>
+      <c r="BU61" s="3"/>
+      <c r="BV61" s="3"/>
+      <c r="BW61" s="3"/>
+      <c r="BX61" s="3"/>
+      <c r="BY61" s="3"/>
+      <c r="BZ61" s="3"/>
+      <c r="CA61" s="3"/>
+      <c r="CB61" s="3"/>
+      <c r="CC61" s="3"/>
+      <c r="CD61" s="3"/>
+      <c r="CE61" s="3"/>
+      <c r="CF61" s="3"/>
+      <c r="CG61" s="3"/>
+      <c r="CH61" s="3"/>
+      <c r="CI61" s="3"/>
+      <c r="CJ61" s="3"/>
+      <c r="CK61" s="3"/>
+      <c r="CL61" s="3"/>
+      <c r="CM61" s="3"/>
+      <c r="CN61" s="3"/>
+      <c r="CO61" s="3"/>
+      <c r="CP61" s="3"/>
+      <c r="CQ61" s="3"/>
+      <c r="CR61" s="3"/>
+      <c r="CS61" s="3"/>
+      <c r="CT61" s="3"/>
+      <c r="CU61" s="3"/>
+      <c r="CV61" s="3"/>
+      <c r="CW61" s="3"/>
+      <c r="CX61" s="3"/>
+      <c r="CY61" s="3"/>
+      <c r="CZ61" s="3"/>
+      <c r="DA61" s="3"/>
+      <c r="DB61" s="3"/>
+    </row>
+    <row r="62" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B62" s="78"/>
+      <c r="C62" s="73"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="65"/>
+      <c r="F62" s="65"/>
+      <c r="G62" s="14"/>
+      <c r="H62" s="14" t="str">
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
-      <c r="I60" s="41"/>
-      <c r="J60" s="41"/>
-      <c r="K60" s="41"/>
-      <c r="L60" s="41"/>
-      <c r="M60" s="41"/>
-      <c r="N60" s="41"/>
-      <c r="O60" s="41"/>
-      <c r="P60" s="41"/>
-      <c r="Q60" s="41"/>
-      <c r="R60" s="41"/>
-      <c r="S60" s="41"/>
-      <c r="T60" s="41"/>
-      <c r="U60" s="41"/>
-      <c r="V60" s="41"/>
-      <c r="W60" s="41"/>
-      <c r="X60" s="41"/>
-      <c r="Y60" s="41"/>
-      <c r="Z60" s="41"/>
-      <c r="AA60" s="41"/>
-      <c r="AB60" s="41"/>
-      <c r="AC60" s="41"/>
-      <c r="AD60" s="41"/>
-      <c r="AE60" s="41"/>
-      <c r="AF60" s="41"/>
-      <c r="AG60" s="41"/>
-      <c r="AH60" s="41"/>
-      <c r="AI60" s="41"/>
-      <c r="AJ60" s="41"/>
-      <c r="AK60" s="41"/>
-      <c r="AL60" s="41"/>
-      <c r="AM60" s="41"/>
-      <c r="AN60" s="41"/>
-      <c r="AO60" s="41"/>
-      <c r="AP60" s="41"/>
-      <c r="AQ60" s="41"/>
-      <c r="AR60" s="41"/>
-      <c r="AS60" s="41"/>
-      <c r="AT60" s="41"/>
-      <c r="AU60" s="41"/>
-      <c r="AV60" s="41"/>
-      <c r="AW60" s="41"/>
-      <c r="AX60" s="41"/>
-      <c r="AY60" s="41"/>
-      <c r="AZ60" s="41"/>
-      <c r="BA60" s="41"/>
-      <c r="BB60" s="41"/>
-      <c r="BC60" s="41"/>
-      <c r="BD60" s="41"/>
-      <c r="BE60" s="41"/>
-      <c r="BF60" s="41"/>
-      <c r="BG60" s="41"/>
-      <c r="BH60" s="41"/>
-      <c r="BI60" s="41"/>
-      <c r="BJ60" s="41"/>
-      <c r="BK60" s="41"/>
-      <c r="BL60" s="41"/>
-      <c r="BM60" s="41"/>
-      <c r="BN60" s="41"/>
-      <c r="BO60" s="41"/>
-      <c r="BP60" s="41"/>
-      <c r="BQ60" s="41"/>
-      <c r="BR60" s="41"/>
-      <c r="BS60" s="41"/>
-      <c r="BT60" s="41"/>
-      <c r="BU60" s="41"/>
-      <c r="BV60" s="41"/>
-      <c r="BW60" s="41"/>
-      <c r="BX60" s="41"/>
-      <c r="BY60" s="41"/>
-      <c r="BZ60" s="41"/>
-      <c r="CA60" s="41"/>
-      <c r="CB60" s="41"/>
-      <c r="CC60" s="41"/>
-      <c r="CD60" s="41"/>
-      <c r="CE60" s="41"/>
-      <c r="CF60" s="41"/>
-      <c r="CG60" s="41"/>
-      <c r="CH60" s="41"/>
-      <c r="CI60" s="41"/>
-      <c r="CJ60" s="41"/>
-      <c r="CK60" s="41"/>
-      <c r="CL60" s="41"/>
-      <c r="CM60" s="41"/>
-      <c r="CN60" s="41"/>
-      <c r="CO60" s="41"/>
-      <c r="CP60" s="41"/>
-      <c r="CQ60" s="41"/>
-      <c r="CR60" s="41"/>
-      <c r="CS60" s="41"/>
-      <c r="CT60" s="41"/>
-      <c r="CU60" s="41"/>
-      <c r="CV60" s="41"/>
-      <c r="CW60" s="41"/>
-      <c r="CX60" s="41"/>
-      <c r="CY60" s="41"/>
-      <c r="CZ60" s="41"/>
-      <c r="DA60" s="41"/>
-      <c r="DB60" s="41"/>
+      <c r="I62" s="41"/>
+      <c r="J62" s="41"/>
+      <c r="K62" s="41"/>
+      <c r="L62" s="41"/>
+      <c r="M62" s="41"/>
+      <c r="N62" s="41"/>
+      <c r="O62" s="41"/>
+      <c r="P62" s="41"/>
+      <c r="Q62" s="41"/>
+      <c r="R62" s="41"/>
+      <c r="S62" s="41"/>
+      <c r="T62" s="41"/>
+      <c r="U62" s="41"/>
+      <c r="V62" s="41"/>
+      <c r="W62" s="41"/>
+      <c r="X62" s="41"/>
+      <c r="Y62" s="41"/>
+      <c r="Z62" s="41"/>
+      <c r="AA62" s="41"/>
+      <c r="AB62" s="41"/>
+      <c r="AC62" s="41"/>
+      <c r="AD62" s="41"/>
+      <c r="AE62" s="41"/>
+      <c r="AF62" s="41"/>
+      <c r="AG62" s="41"/>
+      <c r="AH62" s="41"/>
+      <c r="AI62" s="41"/>
+      <c r="AJ62" s="41"/>
+      <c r="AK62" s="41"/>
+      <c r="AL62" s="41"/>
+      <c r="AM62" s="41"/>
+      <c r="AN62" s="41"/>
+      <c r="AO62" s="41"/>
+      <c r="AP62" s="41"/>
+      <c r="AQ62" s="41"/>
+      <c r="AR62" s="41"/>
+      <c r="AS62" s="41"/>
+      <c r="AT62" s="41"/>
+      <c r="AU62" s="41"/>
+      <c r="AV62" s="41"/>
+      <c r="AW62" s="41"/>
+      <c r="AX62" s="41"/>
+      <c r="AY62" s="41"/>
+      <c r="AZ62" s="41"/>
+      <c r="BA62" s="41"/>
+      <c r="BB62" s="41"/>
+      <c r="BC62" s="41"/>
+      <c r="BD62" s="41"/>
+      <c r="BE62" s="41"/>
+      <c r="BF62" s="41"/>
+      <c r="BG62" s="41"/>
+      <c r="BH62" s="41"/>
+      <c r="BI62" s="41"/>
+      <c r="BJ62" s="41"/>
+      <c r="BK62" s="41"/>
+      <c r="BL62" s="41"/>
+      <c r="BM62" s="41"/>
+      <c r="BN62" s="41"/>
+      <c r="BO62" s="41"/>
+      <c r="BP62" s="41"/>
+      <c r="BQ62" s="41"/>
+      <c r="BR62" s="41"/>
+      <c r="BS62" s="41"/>
+      <c r="BT62" s="41"/>
+      <c r="BU62" s="41"/>
+      <c r="BV62" s="41"/>
+      <c r="BW62" s="41"/>
+      <c r="BX62" s="41"/>
+      <c r="BY62" s="41"/>
+      <c r="BZ62" s="41"/>
+      <c r="CA62" s="41"/>
+      <c r="CB62" s="41"/>
+      <c r="CC62" s="41"/>
+      <c r="CD62" s="41"/>
+      <c r="CE62" s="41"/>
+      <c r="CF62" s="41"/>
+      <c r="CG62" s="41"/>
+      <c r="CH62" s="41"/>
+      <c r="CI62" s="41"/>
+      <c r="CJ62" s="41"/>
+      <c r="CK62" s="41"/>
+      <c r="CL62" s="41"/>
+      <c r="CM62" s="41"/>
+      <c r="CN62" s="41"/>
+      <c r="CO62" s="41"/>
+      <c r="CP62" s="41"/>
+      <c r="CQ62" s="41"/>
+      <c r="CR62" s="41"/>
+      <c r="CS62" s="41"/>
+      <c r="CT62" s="41"/>
+      <c r="CU62" s="41"/>
+      <c r="CV62" s="41"/>
+      <c r="CW62" s="41"/>
+      <c r="CX62" s="41"/>
+      <c r="CY62" s="41"/>
+      <c r="CZ62" s="41"/>
+      <c r="DA62" s="41"/>
+      <c r="DB62" s="41"/>
     </row>
-    <row r="61" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="C61" s="36"/>
-      <c r="D61" s="37"/>
-      <c r="E61" s="38"/>
-      <c r="F61" s="39"/>
-      <c r="G61" s="40"/>
-      <c r="H61" s="40" t="str">
+    <row r="63" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B63" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C63" s="36"/>
+      <c r="D63" s="37"/>
+      <c r="E63" s="38"/>
+      <c r="F63" s="39"/>
+      <c r="G63" s="40"/>
+      <c r="H63" s="40" t="str">
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
-      <c r="I61" s="43"/>
-      <c r="J61" s="43"/>
-      <c r="K61" s="43"/>
-      <c r="L61" s="43"/>
-      <c r="M61" s="43"/>
-      <c r="N61" s="43"/>
-      <c r="O61" s="43"/>
-      <c r="P61" s="43"/>
-      <c r="Q61" s="43"/>
-      <c r="R61" s="43"/>
-      <c r="S61" s="43"/>
-      <c r="T61" s="43"/>
-      <c r="U61" s="43"/>
-      <c r="V61" s="43"/>
-      <c r="W61" s="43"/>
-      <c r="X61" s="43"/>
-      <c r="Y61" s="43"/>
-      <c r="Z61" s="43"/>
-      <c r="AA61" s="43"/>
-      <c r="AB61" s="43"/>
-      <c r="AC61" s="43"/>
-      <c r="AD61" s="43"/>
-      <c r="AE61" s="43"/>
-      <c r="AF61" s="43"/>
-      <c r="AG61" s="43"/>
-      <c r="AH61" s="43"/>
-      <c r="AI61" s="43"/>
-      <c r="AJ61" s="43"/>
-      <c r="AK61" s="43"/>
-      <c r="AL61" s="43"/>
-      <c r="AM61" s="43"/>
-      <c r="AN61" s="43"/>
-      <c r="AO61" s="43"/>
-      <c r="AP61" s="43"/>
-      <c r="AQ61" s="43"/>
-      <c r="AR61" s="43"/>
-      <c r="AS61" s="43"/>
-      <c r="AT61" s="43"/>
-      <c r="AU61" s="43"/>
-      <c r="AV61" s="43"/>
-      <c r="AW61" s="43"/>
-      <c r="AX61" s="43"/>
-      <c r="AY61" s="43"/>
-      <c r="AZ61" s="43"/>
-      <c r="BA61" s="43"/>
-      <c r="BB61" s="43"/>
-      <c r="BC61" s="43"/>
-      <c r="BD61" s="43"/>
-      <c r="BE61" s="43"/>
-      <c r="BF61" s="43"/>
-      <c r="BG61" s="43"/>
-      <c r="BH61" s="43"/>
-      <c r="BI61" s="43"/>
-      <c r="BJ61" s="43"/>
-      <c r="BK61" s="43"/>
-      <c r="BL61" s="43"/>
-      <c r="BM61" s="43"/>
-      <c r="BN61" s="43"/>
-      <c r="BO61" s="43"/>
-      <c r="BP61" s="43"/>
-      <c r="BQ61" s="43"/>
-      <c r="BR61" s="43"/>
-      <c r="BS61" s="43"/>
-      <c r="BT61" s="43"/>
-      <c r="BU61" s="43"/>
-      <c r="BV61" s="43"/>
-      <c r="BW61" s="43"/>
-      <c r="BX61" s="43"/>
-      <c r="BY61" s="43"/>
-      <c r="BZ61" s="43"/>
-      <c r="CA61" s="43"/>
-      <c r="CB61" s="43"/>
-      <c r="CC61" s="43"/>
-      <c r="CD61" s="43"/>
-      <c r="CE61" s="43"/>
-      <c r="CF61" s="43"/>
-      <c r="CG61" s="43"/>
-      <c r="CH61" s="43"/>
-      <c r="CI61" s="43"/>
-      <c r="CJ61" s="43"/>
-      <c r="CK61" s="43"/>
-      <c r="CL61" s="43"/>
-      <c r="CM61" s="43"/>
-      <c r="CN61" s="43"/>
-      <c r="CO61" s="43"/>
-      <c r="CP61" s="43"/>
-      <c r="CQ61" s="43"/>
-      <c r="CR61" s="43"/>
-      <c r="CS61" s="43"/>
-      <c r="CT61" s="43"/>
-      <c r="CU61" s="43"/>
-      <c r="CV61" s="43"/>
-      <c r="CW61" s="43"/>
-      <c r="CX61" s="43"/>
-      <c r="CY61" s="43"/>
-      <c r="CZ61" s="43"/>
-      <c r="DA61" s="43"/>
-      <c r="DB61" s="43"/>
+      <c r="I63" s="43"/>
+      <c r="J63" s="43"/>
+      <c r="K63" s="43"/>
+      <c r="L63" s="43"/>
+      <c r="M63" s="43"/>
+      <c r="N63" s="43"/>
+      <c r="O63" s="43"/>
+      <c r="P63" s="43"/>
+      <c r="Q63" s="43"/>
+      <c r="R63" s="43"/>
+      <c r="S63" s="43"/>
+      <c r="T63" s="43"/>
+      <c r="U63" s="43"/>
+      <c r="V63" s="43"/>
+      <c r="W63" s="43"/>
+      <c r="X63" s="43"/>
+      <c r="Y63" s="43"/>
+      <c r="Z63" s="43"/>
+      <c r="AA63" s="43"/>
+      <c r="AB63" s="43"/>
+      <c r="AC63" s="43"/>
+      <c r="AD63" s="43"/>
+      <c r="AE63" s="43"/>
+      <c r="AF63" s="43"/>
+      <c r="AG63" s="43"/>
+      <c r="AH63" s="43"/>
+      <c r="AI63" s="43"/>
+      <c r="AJ63" s="43"/>
+      <c r="AK63" s="43"/>
+      <c r="AL63" s="43"/>
+      <c r="AM63" s="43"/>
+      <c r="AN63" s="43"/>
+      <c r="AO63" s="43"/>
+      <c r="AP63" s="43"/>
+      <c r="AQ63" s="43"/>
+      <c r="AR63" s="43"/>
+      <c r="AS63" s="43"/>
+      <c r="AT63" s="43"/>
+      <c r="AU63" s="43"/>
+      <c r="AV63" s="43"/>
+      <c r="AW63" s="43"/>
+      <c r="AX63" s="43"/>
+      <c r="AY63" s="43"/>
+      <c r="AZ63" s="43"/>
+      <c r="BA63" s="43"/>
+      <c r="BB63" s="43"/>
+      <c r="BC63" s="43"/>
+      <c r="BD63" s="43"/>
+      <c r="BE63" s="43"/>
+      <c r="BF63" s="43"/>
+      <c r="BG63" s="43"/>
+      <c r="BH63" s="43"/>
+      <c r="BI63" s="43"/>
+      <c r="BJ63" s="43"/>
+      <c r="BK63" s="43"/>
+      <c r="BL63" s="43"/>
+      <c r="BM63" s="43"/>
+      <c r="BN63" s="43"/>
+      <c r="BO63" s="43"/>
+      <c r="BP63" s="43"/>
+      <c r="BQ63" s="43"/>
+      <c r="BR63" s="43"/>
+      <c r="BS63" s="43"/>
+      <c r="BT63" s="43"/>
+      <c r="BU63" s="43"/>
+      <c r="BV63" s="43"/>
+      <c r="BW63" s="43"/>
+      <c r="BX63" s="43"/>
+      <c r="BY63" s="43"/>
+      <c r="BZ63" s="43"/>
+      <c r="CA63" s="43"/>
+      <c r="CB63" s="43"/>
+      <c r="CC63" s="43"/>
+      <c r="CD63" s="43"/>
+      <c r="CE63" s="43"/>
+      <c r="CF63" s="43"/>
+      <c r="CG63" s="43"/>
+      <c r="CH63" s="43"/>
+      <c r="CI63" s="43"/>
+      <c r="CJ63" s="43"/>
+      <c r="CK63" s="43"/>
+      <c r="CL63" s="43"/>
+      <c r="CM63" s="43"/>
+      <c r="CN63" s="43"/>
+      <c r="CO63" s="43"/>
+      <c r="CP63" s="43"/>
+      <c r="CQ63" s="43"/>
+      <c r="CR63" s="43"/>
+      <c r="CS63" s="43"/>
+      <c r="CT63" s="43"/>
+      <c r="CU63" s="43"/>
+      <c r="CV63" s="43"/>
+      <c r="CW63" s="43"/>
+      <c r="CX63" s="43"/>
+      <c r="CY63" s="43"/>
+      <c r="CZ63" s="43"/>
+      <c r="DA63" s="43"/>
+      <c r="DB63" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="CO4:CU4"/>
+    <mergeCell ref="CV4:DB4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="CO4:CU4"/>
-    <mergeCell ref="CV4:DB4"/>
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D60:D61 D7:D57">
+  <conditionalFormatting sqref="D62:D63 D7:D59">
     <cfRule type="dataBar" priority="53">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9516,12 +9782,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I60:BL61 I29:DB57">
+  <conditionalFormatting sqref="I62:BL63 I29:DB59">
     <cfRule type="expression" dxfId="44" priority="72">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I60:BL61 I29:DB57">
+  <conditionalFormatting sqref="I62:BL63 I29:DB59">
     <cfRule type="expression" dxfId="43" priority="66">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -9607,12 +9873,12 @@
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM60:CG61">
+  <conditionalFormatting sqref="BM62:CG63">
     <cfRule type="expression" dxfId="23" priority="21">
       <formula>AND(TODAY()&gt;=BM$5,TODAY()&lt;BN$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM60:CG61">
+  <conditionalFormatting sqref="BM62:CG63">
     <cfRule type="expression" dxfId="22" priority="19">
       <formula>AND(task_start&lt;=BM$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BM$5)</formula>
     </cfRule>
@@ -9659,12 +9925,12 @@
       <formula>AND(task_end&gt;=BM$5,task_start&lt;BN$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CH60:DB61">
+  <conditionalFormatting sqref="CH62:DB63">
     <cfRule type="expression" dxfId="11" priority="9">
       <formula>AND(TODAY()&gt;=CH$5,TODAY()&lt;CI$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CH60:DB61">
+  <conditionalFormatting sqref="CH62:DB63">
     <cfRule type="expression" dxfId="10" priority="7">
       <formula>AND(task_start&lt;=CH$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CH$5)</formula>
     </cfRule>
@@ -9711,17 +9977,20 @@
       <formula>AND(task_end&gt;=CH$5,task_start&lt;CI$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Changing this number will scroll the Gantt Chart view." sqref="E4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>1</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35433070866141736" right="0.35433070866141736" top="0.35433070866141736" bottom="0.51181102362204722" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="8" scale="57" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="8" scale="41" fitToHeight="160" orientation="landscape" r:id="rId1"/>
   <headerFooter differentFirst="1" scaleWithDoc="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="61" max="16383" man="1"/>
+  </rowBreaks>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -9738,7 +10007,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D60:D61 D7:D57</xm:sqref>
+          <xm:sqref>D62:D63 D7:D59</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -9761,79 +10030,79 @@
     <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:2" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="46" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B2" s="46"/>
     </row>
     <row r="3" spans="1:2" s="51" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="82" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B3" s="52"/>
     </row>
     <row r="4" spans="1:2" s="48" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A4" s="49" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="50" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="49" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="45" customFormat="1" ht="205.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="54" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="48" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A8" s="49" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="50" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="45" customFormat="1" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="53" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="48" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A11" s="49" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="50" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="45" customFormat="1" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="53" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="48" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A14" s="49" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="50" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="50" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -9850,15 +10119,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F460D63BE02C844ABCDAE95AC4045663" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="168d45809451272d4eab4000d1faa223">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3c7e7f14-e12e-4011-a8f5-4b5c28e9eb09" xmlns:ns3="023e2482-3843-4ba8-8468-8ccd9ac81216" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c940773947e86160656b2c3c86f1dd6c" ns2:_="" ns3:_="">
     <xsd:import namespace="3c7e7f14-e12e-4011-a8f5-4b5c28e9eb09"/>
@@ -10101,15 +10361,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D004AD92-7D8D-4284-9E4A-75773209AD85}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1A2F4BF-64F9-49C3-913A-DEDB0A7FC48A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10126,4 +10387,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D004AD92-7D8D-4284-9E4A-75773209AD85}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added to the documents
Finished with the Gantt chart in the organisational document and added the wireframe and storyboard to the technical document.
</commit_message>
<xml_diff>
--- a/Rampage/Rampage Gantt Chart.xlsx
+++ b/Rampage/Rampage Gantt Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B29C99-62C7-44FD-B6A3-FE4DADCC1107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EAE9B7D-A415-4449-9958-35208739595A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -316,9 +316,6 @@
     <t>Leaderboard</t>
   </si>
   <si>
-    <t>NPCS/ Building, Main Playing Scene</t>
-  </si>
-  <si>
     <t xml:space="preserve">Testing </t>
   </si>
   <si>
@@ -329,6 +326,9 @@
   </si>
   <si>
     <t>Menus, Audio</t>
+  </si>
+  <si>
+    <t>NPCS/ Buildings, Main Playing Scene</t>
   </si>
 </sst>
 </file>
@@ -1996,8 +1996,8 @@
   <dimension ref="A1:DB63"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="60" zoomScaleNormal="60" zoomScaleSheetLayoutView="59" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AP31" sqref="AP31"/>
+      <pane ySplit="6" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7889,7 +7889,7 @@
         <v>46</v>
       </c>
       <c r="D48" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E48" s="88">
         <f>Project_Start+ 74</f>
@@ -8127,10 +8127,10 @@
         <v>75</v>
       </c>
       <c r="C50" s="87" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D50" s="34">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="E50" s="64">
         <f>Project_Start+87</f>
@@ -8243,13 +8243,13 @@
     </row>
     <row r="51" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B51" s="86" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C51" s="87" t="s">
         <v>60</v>
       </c>
       <c r="D51" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E51" s="64">
         <f>Project_Start+87</f>
@@ -8368,7 +8368,7 @@
         <v>57</v>
       </c>
       <c r="D52" s="34">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E52" s="64">
         <f>Project_Start+ 63</f>
@@ -8487,7 +8487,7 @@
         <v>59</v>
       </c>
       <c r="D53" s="34">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E53" s="64">
         <f>Project_Start+64</f>
@@ -8600,13 +8600,13 @@
     </row>
     <row r="54" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B54" s="86" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C54" s="87" t="s">
         <v>65</v>
       </c>
       <c r="D54" s="34">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E54" s="64">
         <f>Project_Start+ 63</f>
@@ -8719,13 +8719,13 @@
     </row>
     <row r="55" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B55" s="86" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C55" s="87" t="s">
         <v>46</v>
       </c>
       <c r="D55" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E55" s="64">
         <f>Project_Start+92</f>
@@ -8838,13 +8838,13 @@
     </row>
     <row r="56" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B56" s="86" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C56" s="87" t="s">
         <v>46</v>
       </c>
       <c r="D56" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E56" s="64">
         <f>Project_Start+92</f>
@@ -8963,10 +8963,10 @@
         <v>42</v>
       </c>
       <c r="C57" s="87" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D57" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E57" s="64">
         <f>Project_Start+92</f>
@@ -9088,7 +9088,7 @@
         <v>46</v>
       </c>
       <c r="D58" s="34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E58" s="64">
         <f>Project_Start+92</f>

</xml_diff>